<commit_message>
Improve forecast accuracy: last 30d only, drop top 1% outliers, log-transform, add moving average baseline, add warning if forecast is too high. Update README with 'for dummies' section and formulas.
</commit_message>
<xml_diff>
--- a/forecast_results.xlsx
+++ b/forecast_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E218"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,13 +474,13 @@
         <v>45767</v>
       </c>
       <c r="C2" t="n">
-        <v>29.67653806315084</v>
+        <v>60.76824678643709</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>17.92156318875243</v>
       </c>
       <c r="E2" t="n">
-        <v>71.91464298817003</v>
+        <v>103.5784422748278</v>
       </c>
     </row>
     <row r="3">
@@ -493,13 +493,13 @@
         <v>45768</v>
       </c>
       <c r="C3" t="n">
-        <v>48.62963963917623</v>
+        <v>98.86408184770652</v>
       </c>
       <c r="D3" t="n">
-        <v>3.396306625043896</v>
+        <v>55.3028162081028</v>
       </c>
       <c r="E3" t="n">
-        <v>96.04866809167387</v>
+        <v>142.9303026368978</v>
       </c>
     </row>
     <row r="4">
@@ -512,13 +512,13 @@
         <v>45769</v>
       </c>
       <c r="C4" t="n">
-        <v>36.09962977429412</v>
+        <v>108.6743532324353</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>66.98284500042551</v>
       </c>
       <c r="E4" t="n">
-        <v>80.14778014196513</v>
+        <v>149.3122734864707</v>
       </c>
     </row>
     <row r="5">
@@ -531,13 +531,13 @@
         <v>45770</v>
       </c>
       <c r="C5" t="n">
-        <v>31.59034450026116</v>
+        <v>128.2616842309874</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>86.94517279329133</v>
       </c>
       <c r="E5" t="n">
-        <v>80.32246213308365</v>
+        <v>169.2234913125083</v>
       </c>
     </row>
     <row r="6">
@@ -550,13 +550,13 @@
         <v>45771</v>
       </c>
       <c r="C6" t="n">
-        <v>32.17561610712968</v>
+        <v>165.6364228892348</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>123.2326884091502</v>
       </c>
       <c r="E6" t="n">
-        <v>77.11893894042534</v>
+        <v>208.2131915785384</v>
       </c>
     </row>
     <row r="7">
@@ -569,13 +569,13 @@
         <v>45772</v>
       </c>
       <c r="C7" t="n">
-        <v>36.50262247322555</v>
+        <v>188.076768549791</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>143.3858631599797</v>
       </c>
       <c r="E7" t="n">
-        <v>82.35127041796328</v>
+        <v>231.1407393767046</v>
       </c>
     </row>
     <row r="8">
@@ -588,13 +588,13 @@
         <v>45773</v>
       </c>
       <c r="C8" t="n">
-        <v>42.68605060095268</v>
+        <v>241.9233551810334</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>196.219411290455</v>
       </c>
       <c r="E8" t="n">
-        <v>90.17024202215202</v>
+        <v>283.0168343550589</v>
       </c>
     </row>
     <row r="9">
@@ -607,13 +607,13 @@
         <v>45766</v>
       </c>
       <c r="C9" t="n">
-        <v>129.7507387029984</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>303.0190204790943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -626,13 +626,13 @@
         <v>45767</v>
       </c>
       <c r="C10" t="n">
-        <v>121.7312764404443</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>293.5147584489331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -645,13 +645,13 @@
         <v>45768</v>
       </c>
       <c r="C11" t="n">
-        <v>83.99148812194987</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>263.919098303602</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -664,13 +664,13 @@
         <v>45769</v>
       </c>
       <c r="C12" t="n">
-        <v>75.57324505284296</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>246.6139253252737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -683,13 +683,13 @@
         <v>45770</v>
       </c>
       <c r="C13" t="n">
-        <v>77.48910150229146</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>259.5434095793839</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -702,13 +702,13 @@
         <v>45771</v>
       </c>
       <c r="C14" t="n">
-        <v>45.77908307679799</v>
+        <v>810.7736074693294</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>810.7736074239187</v>
       </c>
       <c r="E14" t="n">
-        <v>228.4357577049093</v>
+        <v>810.7736075199472</v>
       </c>
     </row>
     <row r="15">
@@ -721,13 +721,13 @@
         <v>45772</v>
       </c>
       <c r="C15" t="n">
-        <v>53.41018617976646</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>234.687577368687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -740,13 +740,13 @@
         <v>45766</v>
       </c>
       <c r="C16" t="n">
-        <v>15.73745573290266</v>
+        <v>50.90917922207742</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>50.90896178839044</v>
       </c>
       <c r="E16" t="n">
-        <v>33.29488148892595</v>
+        <v>50.9094030220986</v>
       </c>
     </row>
     <row r="17">
@@ -759,13 +759,13 @@
         <v>45767</v>
       </c>
       <c r="C17" t="n">
-        <v>20.05806586475245</v>
+        <v>95.50472580526795</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6114647541444067</v>
+        <v>95.50372137465051</v>
       </c>
       <c r="E17" t="n">
-        <v>39.0446618088004</v>
+        <v>95.50616717210939</v>
       </c>
     </row>
     <row r="18">
@@ -778,13 +778,13 @@
         <v>45768</v>
       </c>
       <c r="C18" t="n">
-        <v>13.77050006483665</v>
+        <v>103.9993025184341</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>103.9970549566478</v>
       </c>
       <c r="E18" t="n">
-        <v>32.43676932930985</v>
+        <v>104.0023419803772</v>
       </c>
     </row>
     <row r="19">
@@ -797,13 +797,13 @@
         <v>45769</v>
       </c>
       <c r="C19" t="n">
-        <v>22.23299807596458</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>4.711019946543041</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>40.52589234348531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -816,13 +816,13 @@
         <v>45770</v>
       </c>
       <c r="C20" t="n">
-        <v>19.23212055259777</v>
+        <v>505.3209580228585</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>505.3153671037848</v>
       </c>
       <c r="E20" t="n">
-        <v>38.11241202531037</v>
+        <v>505.3277769398213</v>
       </c>
     </row>
     <row r="21">
@@ -835,13 +835,13 @@
         <v>45771</v>
       </c>
       <c r="C21" t="n">
-        <v>18.37412285932963</v>
+        <v>698.1809680400684</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1891650388568559</v>
+        <v>698.1735292122618</v>
       </c>
       <c r="E21" t="n">
-        <v>37.39187482963441</v>
+        <v>698.1900596538532</v>
       </c>
     </row>
     <row r="22">
@@ -854,13 +854,13 @@
         <v>45772</v>
       </c>
       <c r="C22" t="n">
-        <v>22.06388749539962</v>
+        <v>541.9476261092277</v>
       </c>
       <c r="D22" t="n">
-        <v>4.468369246845904</v>
+        <v>541.9370937146657</v>
       </c>
       <c r="E22" t="n">
-        <v>39.56248467223786</v>
+        <v>541.9590332887175</v>
       </c>
     </row>
     <row r="23">
@@ -873,13 +873,13 @@
         <v>45767</v>
       </c>
       <c r="C23" t="n">
-        <v>31.41751725095139</v>
+        <v>263.2003711919922</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>263.1438855615921</v>
       </c>
       <c r="E23" t="n">
-        <v>90.90213211822081</v>
+        <v>263.3298975393203</v>
       </c>
     </row>
     <row r="24">
@@ -892,13 +892,13 @@
         <v>45768</v>
       </c>
       <c r="C24" t="n">
-        <v>1.60354216397605</v>
+        <v>136.0397238315839</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>135.7359092230663</v>
       </c>
       <c r="E24" t="n">
-        <v>62.98300513054667</v>
+        <v>136.4571888351116</v>
       </c>
     </row>
     <row r="25">
@@ -911,13 +911,13 @@
         <v>45769</v>
       </c>
       <c r="C25" t="n">
-        <v>22.61345460152135</v>
+        <v>184.2084641863586</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>183.4632646856033</v>
       </c>
       <c r="E25" t="n">
-        <v>86.07859671252494</v>
+        <v>185.2221268429114</v>
       </c>
     </row>
     <row r="26">
@@ -930,13 +930,13 @@
         <v>45770</v>
       </c>
       <c r="C26" t="n">
-        <v>23.13071014099109</v>
+        <v>438.2769869364718</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>436.956863350859</v>
       </c>
       <c r="E26" t="n">
-        <v>83.77027781987489</v>
+        <v>440.0791506738954</v>
       </c>
     </row>
     <row r="27">
@@ -949,13 +949,13 @@
         <v>45771</v>
       </c>
       <c r="C27" t="n">
-        <v>21.8075748508162</v>
+        <v>403.845249742175</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>402.10761395976</v>
       </c>
       <c r="E27" t="n">
-        <v>81.09104511677856</v>
+        <v>406.2972290634654</v>
       </c>
     </row>
     <row r="28">
@@ -968,13 +968,13 @@
         <v>45772</v>
       </c>
       <c r="C28" t="n">
-        <v>40.64004397593142</v>
+        <v>582.6073699133352</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>580.1810908985439</v>
       </c>
       <c r="E28" t="n">
-        <v>103.5728949445207</v>
+        <v>585.8252035925431</v>
       </c>
     </row>
     <row r="29">
@@ -987,13 +987,13 @@
         <v>45773</v>
       </c>
       <c r="C29" t="n">
-        <v>24.25627362804233</v>
+        <v>413.0978751847587</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>409.8092352112416</v>
       </c>
       <c r="E29" t="n">
-        <v>82.74502774214616</v>
+        <v>417.2147431438697</v>
       </c>
     </row>
     <row r="30">
@@ -1006,13 +1006,13 @@
         <v>45765</v>
       </c>
       <c r="C30" t="n">
-        <v>75.3006596574885</v>
+        <v>256.7281118152473</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>256.6607355418666</v>
       </c>
       <c r="E30" t="n">
-        <v>175.3183223076191</v>
+        <v>256.8093688043152</v>
       </c>
     </row>
     <row r="31">
@@ -1025,13 +1025,13 @@
         <v>45766</v>
       </c>
       <c r="C31" t="n">
-        <v>64.20908785662175</v>
+        <v>188.988662196341</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>188.7291195485863</v>
       </c>
       <c r="E31" t="n">
-        <v>145.8113051816362</v>
+        <v>189.2340662581526</v>
       </c>
     </row>
     <row r="32">
@@ -1044,13 +1044,13 @@
         <v>45767</v>
       </c>
       <c r="C32" t="n">
-        <v>75.86028009685663</v>
+        <v>122.0468051365797</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>121.441092242768</v>
       </c>
       <c r="E32" t="n">
-        <v>166.3304207796507</v>
+        <v>122.5291184180281</v>
       </c>
     </row>
     <row r="33">
@@ -1063,13 +1063,13 @@
         <v>45768</v>
       </c>
       <c r="C33" t="n">
-        <v>79.47052343373525</v>
+        <v>73.88780453966069</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>72.87842356800708</v>
       </c>
       <c r="E33" t="n">
-        <v>175.9088274212353</v>
+        <v>74.69602748372543</v>
       </c>
     </row>
     <row r="34">
@@ -1082,13 +1082,13 @@
         <v>45769</v>
       </c>
       <c r="C34" t="n">
-        <v>56.6744849962048</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>153.8535207729418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1101,13 +1101,13 @@
         <v>45770</v>
       </c>
       <c r="C35" t="n">
-        <v>28.61447502386136</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>133.7782679150949</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1120,213 +1120,213 @@
         <v>45771</v>
       </c>
       <c r="C36" t="n">
-        <v>9.852841630146031</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>106.9733490822611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45608</v>
+        <v>45744</v>
       </c>
       <c r="C37" t="n">
-        <v>2.528787124952216</v>
+        <v>11.69036590716986</v>
       </c>
       <c r="D37" t="n">
-        <v>2.188953750418505</v>
+        <v>11.67488965078122</v>
       </c>
       <c r="E37" t="n">
-        <v>2.856377105629531</v>
+        <v>11.69988732035373</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45609</v>
+        <v>45745</v>
       </c>
       <c r="C38" t="n">
-        <v>2.219155504634583</v>
+        <v>50.68382159093581</v>
       </c>
       <c r="D38" t="n">
-        <v>1.879937295227103</v>
+        <v>50.63536501774212</v>
       </c>
       <c r="E38" t="n">
-        <v>2.557986587561746</v>
+        <v>50.72367194760093</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45610</v>
+        <v>45746</v>
       </c>
       <c r="C39" t="n">
-        <v>2.800480377740077</v>
+        <v>16.65335221923896</v>
       </c>
       <c r="D39" t="n">
-        <v>2.470769025046655</v>
+        <v>16.55302011098445</v>
       </c>
       <c r="E39" t="n">
-        <v>3.111454479431969</v>
+        <v>16.72799987878723</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45611</v>
+        <v>45747</v>
       </c>
       <c r="C40" t="n">
-        <v>3.646608882323624</v>
+        <v>56.25714178977801</v>
       </c>
       <c r="D40" t="n">
-        <v>3.29296308623658</v>
+        <v>56.10148081973866</v>
       </c>
       <c r="E40" t="n">
-        <v>3.989379577162197</v>
+        <v>56.37392893872373</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45612</v>
+        <v>45748</v>
       </c>
       <c r="C41" t="n">
-        <v>2.669243831981124</v>
+        <v>215.8595403123659</v>
       </c>
       <c r="D41" t="n">
-        <v>2.338147020396016</v>
+        <v>215.6428429231771</v>
       </c>
       <c r="E41" t="n">
-        <v>2.995392595619667</v>
+        <v>216.0342278051884</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45613</v>
+        <v>45749</v>
       </c>
       <c r="C42" t="n">
-        <v>20.37223811577933</v>
+        <v>13.68471782364635</v>
       </c>
       <c r="D42" t="n">
-        <v>20.03785840446989</v>
+        <v>13.41856505947631</v>
       </c>
       <c r="E42" t="n">
-        <v>20.70424479448254</v>
+        <v>13.91013988190961</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>taxi bike</t>
+          <t>subscriptions</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45614</v>
+        <v>45750</v>
       </c>
       <c r="C43" t="n">
-        <v>4.012195709359735</v>
+        <v>23.17835981018209</v>
       </c>
       <c r="D43" t="n">
-        <v>3.686140881341483</v>
+        <v>22.84827497726198</v>
       </c>
       <c r="E43" t="n">
-        <v>4.354176361727852</v>
+        <v>23.4768699619408</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45744</v>
+        <v>45708</v>
       </c>
       <c r="C44" t="n">
-        <v>12.53370936486533</v>
+        <v>13.62573263617267</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>13.62573260673272</v>
       </c>
       <c r="E44" t="n">
-        <v>25.93939287138359</v>
+        <v>13.62573266740913</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45745</v>
+        <v>45709</v>
       </c>
       <c r="C45" t="n">
-        <v>23.8207155328181</v>
+        <v>10.78686582995319</v>
       </c>
       <c r="D45" t="n">
-        <v>9.821401658253681</v>
+        <v>10.7868657578142</v>
       </c>
       <c r="E45" t="n">
-        <v>38.17538772239247</v>
+        <v>10.78686591583241</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45746</v>
+        <v>45710</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>5.83512585174555</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>5.835125709090917</v>
       </c>
       <c r="E46" t="n">
-        <v>11.0847829829343</v>
+        <v>5.835126006452025</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45747</v>
+        <v>45711</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -1335,17 +1335,17 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>11.93746827866093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45748</v>
+        <v>45712</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -1354,17 +1354,17 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>1.514605936868496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45749</v>
+        <v>45713</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -1379,11 +1379,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>subscriptions</t>
+          <t>taxi car</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45750</v>
+        <v>45714</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -1398,562 +1398,562 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45708</v>
+        <v>45766</v>
       </c>
       <c r="C51" t="n">
-        <v>5.753966223829933</v>
+        <v>19.37821246898756</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>16.81307216690037</v>
+        <v>46.99636324037575</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45709</v>
+        <v>45767</v>
       </c>
       <c r="C52" t="n">
-        <v>5.128925080071864</v>
+        <v>13.26848198230812</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>15.96440383407519</v>
+        <v>45.09741091891934</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45710</v>
+        <v>45768</v>
       </c>
       <c r="C53" t="n">
-        <v>4.45162466235772</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>16.12018945397245</v>
+        <v>22.69143121166511</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>45711</v>
+        <v>45769</v>
       </c>
       <c r="C54" t="n">
-        <v>3.708036281313914</v>
+        <v>6.329027763023305</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>15.3630777168841</v>
+        <v>34.93013709632029</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
-        <v>45712</v>
+        <v>45770</v>
       </c>
       <c r="C55" t="n">
-        <v>2.612714558502207</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>14.50953845868988</v>
+        <v>0.1287104646499408</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45713</v>
+        <v>45771</v>
       </c>
       <c r="C56" t="n">
-        <v>3.900610145490119</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>15.55804213757955</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>taxi car</t>
+          <t>cafes</t>
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45714</v>
+        <v>45772</v>
       </c>
       <c r="C57" t="n">
-        <v>2.922965876012134</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>13.71234891656437</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>45766</v>
+        <v>45767</v>
       </c>
       <c r="C58" t="n">
-        <v>33.59103991654528</v>
+        <v>48.11491934781691</v>
       </c>
       <c r="D58" t="n">
-        <v>8.224957745780204</v>
+        <v>48.11491930137817</v>
       </c>
       <c r="E58" t="n">
-        <v>56.96895887979285</v>
+        <v>48.11491939182399</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>45767</v>
+        <v>45768</v>
       </c>
       <c r="C59" t="n">
-        <v>35.14832018872885</v>
+        <v>55.9493248264255</v>
       </c>
       <c r="D59" t="n">
-        <v>12.09954673297186</v>
+        <v>55.94932478318142</v>
       </c>
       <c r="E59" t="n">
-        <v>59.30416488588647</v>
+        <v>55.94932486870866</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B60" s="2" t="n">
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="C60" t="n">
-        <v>17.56507902942276</v>
+        <v>63.11361350375644</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>63.11361345950887</v>
       </c>
       <c r="E60" t="n">
-        <v>41.09014957158697</v>
+        <v>63.1136135484036</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B61" s="2" t="n">
-        <v>45769</v>
+        <v>45770</v>
       </c>
       <c r="C61" t="n">
-        <v>25.72212433428782</v>
+        <v>69.6203545987287</v>
       </c>
       <c r="D61" t="n">
-        <v>0.6963596000328628</v>
+        <v>69.62035455751248</v>
       </c>
       <c r="E61" t="n">
-        <v>50.39306902683814</v>
+        <v>69.62035464358065</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B62" s="2" t="n">
-        <v>45770</v>
+        <v>45771</v>
       </c>
       <c r="C62" t="n">
-        <v>22.99708445548355</v>
+        <v>75.46485395840855</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>75.46485391761075</v>
       </c>
       <c r="E62" t="n">
-        <v>48.90534647131222</v>
+        <v>75.46485400389609</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B63" s="2" t="n">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="C63" t="n">
-        <v>21.67089065246672</v>
+        <v>80.62736592148997</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>80.62736587523906</v>
       </c>
       <c r="E63" t="n">
-        <v>47.18716148537356</v>
+        <v>80.62736596595784</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>cafes</t>
+          <t>fun</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
-        <v>45772</v>
+        <v>45773</v>
       </c>
       <c r="C64" t="n">
-        <v>27.44329278113054</v>
+        <v>85.0764952666932</v>
       </c>
       <c r="D64" t="n">
-        <v>2.392615098258571</v>
+        <v>85.07649522215104</v>
       </c>
       <c r="E64" t="n">
-        <v>53.13574465198635</v>
+        <v>85.07649531457068</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B65" s="2" t="n">
-        <v>45448</v>
+        <v>45763</v>
       </c>
       <c r="C65" t="n">
-        <v>8.628611324817776</v>
+        <v>399</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>398.999999212916</v>
       </c>
       <c r="E65" t="n">
-        <v>27.2047391297667</v>
+        <v>399.0000007745616</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
-        <v>45449</v>
+        <v>45764</v>
       </c>
       <c r="C66" t="n">
-        <v>13.19991186415707</v>
+        <v>399</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>398.9999992196296</v>
       </c>
       <c r="E66" t="n">
-        <v>32.48084016909571</v>
+        <v>399.0000008101568</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B67" s="2" t="n">
-        <v>45450</v>
+        <v>45765</v>
       </c>
       <c r="C67" t="n">
-        <v>11.80383201759819</v>
+        <v>399</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>398.9999992336313</v>
       </c>
       <c r="E67" t="n">
-        <v>29.66129277953924</v>
+        <v>399.0000007898352</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
-        <v>45451</v>
+        <v>45766</v>
       </c>
       <c r="C68" t="n">
-        <v>9.772529397302423</v>
+        <v>399</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>398.9999992419957</v>
       </c>
       <c r="E68" t="n">
-        <v>28.15057112100163</v>
+        <v>399.0000008294877</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
-        <v>45452</v>
+        <v>45767</v>
       </c>
       <c r="C69" t="n">
-        <v>9.180927051727426</v>
+        <v>399</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>398.9999992318361</v>
       </c>
       <c r="E69" t="n">
-        <v>25.70566702339733</v>
+        <v>399.0000008491054</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B70" s="2" t="n">
-        <v>45453</v>
+        <v>45768</v>
       </c>
       <c r="C70" t="n">
-        <v>3.024588806038251</v>
+        <v>399</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>398.9999992009765</v>
       </c>
       <c r="E70" t="n">
-        <v>21.69335032137647</v>
+        <v>399.0000007972122</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>groceries + alco</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
-        <v>45454</v>
+        <v>45769</v>
       </c>
       <c r="C71" t="n">
-        <v>6.590936234134821</v>
+        <v>399</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>398.9999991903171</v>
       </c>
       <c r="E71" t="n">
-        <v>24.51419088183999</v>
+        <v>399.0000008388249</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
-        <v>45767</v>
+        <v>45766</v>
       </c>
       <c r="C72" t="n">
-        <v>51.70829663839169</v>
+        <v>56.33612392448998</v>
       </c>
       <c r="D72" t="n">
-        <v>24.65689952665404</v>
+        <v>56.33612387213181</v>
       </c>
       <c r="E72" t="n">
-        <v>76.90194907202505</v>
+        <v>56.33612397089891</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
-        <v>45768</v>
+        <v>45767</v>
       </c>
       <c r="C73" t="n">
-        <v>59.97641954872641</v>
+        <v>60.65772604391186</v>
       </c>
       <c r="D73" t="n">
-        <v>35.02576055084194</v>
+        <v>60.6577259948001</v>
       </c>
       <c r="E73" t="n">
-        <v>87.02037407978479</v>
+        <v>60.6577260858888</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
-        <v>45769</v>
+        <v>45768</v>
       </c>
       <c r="C74" t="n">
-        <v>62.58441150067875</v>
+        <v>62.68487430970997</v>
       </c>
       <c r="D74" t="n">
-        <v>39.33630743533103</v>
+        <v>62.68487426202618</v>
       </c>
       <c r="E74" t="n">
-        <v>88.16357031407831</v>
+        <v>62.68487436214999</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
-        <v>45770</v>
+        <v>45769</v>
       </c>
       <c r="C75" t="n">
-        <v>73.31805954904604</v>
+        <v>62.30142347522046</v>
       </c>
       <c r="D75" t="n">
-        <v>48.34860065294041</v>
+        <v>62.30142342533742</v>
       </c>
       <c r="E75" t="n">
-        <v>98.50227690005703</v>
+        <v>62.30142352200838</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
-        <v>45771</v>
+        <v>45770</v>
       </c>
       <c r="C76" t="n">
-        <v>77.02842105397839</v>
+        <v>59.45787003075235</v>
       </c>
       <c r="D76" t="n">
-        <v>50.15601544129115</v>
+        <v>59.45786998349089</v>
       </c>
       <c r="E76" t="n">
-        <v>103.1490535413849</v>
+        <v>59.45787007865151</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
-        <v>45772</v>
+        <v>45771</v>
       </c>
       <c r="C77" t="n">
-        <v>77.1275116666348</v>
+        <v>54.17239877349708</v>
       </c>
       <c r="D77" t="n">
-        <v>54.55457515237442</v>
+        <v>54.17239872231968</v>
       </c>
       <c r="E77" t="n">
-        <v>103.4818941409204</v>
+        <v>54.17239882758812</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>fun</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
-        <v>45773</v>
+        <v>45772</v>
       </c>
       <c r="C78" t="n">
-        <v>70.2012507495503</v>
+        <v>46.5299822781121</v>
       </c>
       <c r="D78" t="n">
-        <v>44.13021880778764</v>
+        <v>46.52998222707347</v>
       </c>
       <c r="E78" t="n">
-        <v>95.64327550197788</v>
+        <v>46.52998233179729</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
-        <v>45763</v>
+        <v>45684</v>
       </c>
       <c r="C79" t="n">
-        <v>163.1240006269887</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>535.4128398591021</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
-        <v>45764</v>
+        <v>45685</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
@@ -1962,17 +1962,17 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>281.4280044555832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
-        <v>45765</v>
+        <v>45686</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
@@ -1981,17 +1981,17 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>36.83568592085533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
-        <v>45766</v>
+        <v>45687</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
@@ -2006,11 +2006,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
-        <v>45767</v>
+        <v>45688</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
@@ -2025,11 +2025,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
-        <v>45768</v>
+        <v>45689</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
@@ -2044,11 +2044,11 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>steam&amp;PS&amp;Google play</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
-        <v>45769</v>
+        <v>45690</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
@@ -2063,121 +2063,121 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
         <v>45766</v>
       </c>
       <c r="C86" t="n">
-        <v>19.76779392530881</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>19.7677938919271</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>19.767793958441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
         <v>45767</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1358.985685728551</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>1358.985685716031</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1358.985685749218</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B88" s="2" t="n">
         <v>45768</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>701.4154471976088</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>701.4154471487151</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>701.4154472728964</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B89" s="2" t="n">
         <v>45769</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>1695.83959558081</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>1695.839595473938</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>1695.839595729794</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
         <v>45770</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>1238.755601601442</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1238.755601407548</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>1238.755601841836</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
         <v>45771</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>1306.321670247206</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>1306.321669915092</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>1306.32167058202</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>clothes</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
@@ -2196,581 +2196,581 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
-        <v>45682</v>
+        <v>45766</v>
       </c>
       <c r="C93" t="n">
-        <v>106.8009257078589</v>
+        <v>6.225711331245121</v>
       </c>
       <c r="D93" t="n">
-        <v>106.8009255061188</v>
+        <v>6.22571131719886</v>
       </c>
       <c r="E93" t="n">
-        <v>106.8009259022266</v>
+        <v>6.225711343508322</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B94" s="2" t="n">
-        <v>45683</v>
+        <v>45767</v>
       </c>
       <c r="C94" t="n">
-        <v>14.46099916907214</v>
+        <v>2.224211845131506</v>
       </c>
       <c r="D94" t="n">
-        <v>14.46099897959604</v>
+        <v>2.224211831504274</v>
       </c>
       <c r="E94" t="n">
-        <v>14.46099936775595</v>
+        <v>2.224211859492205</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B95" s="2" t="n">
-        <v>45684</v>
+        <v>45768</v>
       </c>
       <c r="C95" t="n">
-        <v>434.8900583796363</v>
+        <v>0.1026521586141631</v>
       </c>
       <c r="D95" t="n">
-        <v>434.890058188898</v>
+        <v>0.1026521441486343</v>
       </c>
       <c r="E95" t="n">
-        <v>434.890058574061</v>
+        <v>0.1026521721712645</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B96" s="2" t="n">
-        <v>45685</v>
+        <v>45769</v>
       </c>
       <c r="C96" t="n">
-        <v>795.221006859405</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>795.2210066501481</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>795.2210070560144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B97" s="2" t="n">
-        <v>45686</v>
+        <v>45770</v>
       </c>
       <c r="C97" t="n">
-        <v>83.43039607693721</v>
+        <v>1.734283532890765</v>
       </c>
       <c r="D97" t="n">
-        <v>83.43039587482365</v>
+        <v>1.734283518584336</v>
       </c>
       <c r="E97" t="n">
-        <v>83.43039627167906</v>
+        <v>1.734283547021723</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B98" s="2" t="n">
-        <v>45687</v>
+        <v>45771</v>
       </c>
       <c r="C98" t="n">
-        <v>578.991521514555</v>
+        <v>5.506961729240553</v>
       </c>
       <c r="D98" t="n">
-        <v>578.9915213219815</v>
+        <v>5.506961713930207</v>
       </c>
       <c r="E98" t="n">
-        <v>578.9915217090771</v>
+        <v>5.506961743086712</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>hotel accomondation and fun</t>
+          <t>phone, internet</t>
         </is>
       </c>
       <c r="B99" s="2" t="n">
-        <v>45688</v>
+        <v>45772</v>
       </c>
       <c r="C99" t="n">
-        <v>688.499879262549</v>
+        <v>11.199502390283</v>
       </c>
       <c r="D99" t="n">
-        <v>688.4998790707238</v>
+        <v>11.19950237474428</v>
       </c>
       <c r="E99" t="n">
-        <v>688.4998794551411</v>
+        <v>11.1995024044851</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B100" s="2" t="n">
-        <v>45684</v>
+        <v>45766</v>
       </c>
       <c r="C100" t="n">
-        <v>77.10770213076866</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>57.863877440839</v>
+        <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>95.48405107286953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B101" s="2" t="n">
-        <v>45685</v>
+        <v>45767</v>
       </c>
       <c r="C101" t="n">
-        <v>34.62872888256747</v>
+        <v>255.0066200804224</v>
       </c>
       <c r="D101" t="n">
-        <v>17.07464323884725</v>
+        <v>255.0066196532995</v>
       </c>
       <c r="E101" t="n">
-        <v>52.2701712146272</v>
+        <v>255.0066204870999</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B102" s="2" t="n">
-        <v>45686</v>
+        <v>45768</v>
       </c>
       <c r="C102" t="n">
-        <v>56.93050513629913</v>
+        <v>88.04623630758738</v>
       </c>
       <c r="D102" t="n">
-        <v>38.23420707780368</v>
+        <v>88.04623534319354</v>
       </c>
       <c r="E102" t="n">
-        <v>75.07219735468574</v>
+        <v>88.04623716868578</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B103" s="2" t="n">
-        <v>45687</v>
+        <v>45769</v>
       </c>
       <c r="C103" t="n">
-        <v>15.00782112122799</v>
+        <v>560.2119744683562</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>560.2119730521913</v>
       </c>
       <c r="E103" t="n">
-        <v>33.27750683926615</v>
+        <v>560.2119759917342</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B104" s="2" t="n">
-        <v>45688</v>
+        <v>45770</v>
       </c>
       <c r="C104" t="n">
-        <v>24.41054145079691</v>
+        <v>447.1125724755398</v>
       </c>
       <c r="D104" t="n">
-        <v>5.465238516860956</v>
+        <v>447.1125702660622</v>
       </c>
       <c r="E104" t="n">
-        <v>43.31647481404467</v>
+        <v>447.1125747254862</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B105" s="2" t="n">
-        <v>45689</v>
+        <v>45771</v>
       </c>
       <c r="C105" t="n">
-        <v>53.28800926560938</v>
+        <v>2013.904669763425</v>
       </c>
       <c r="D105" t="n">
-        <v>35.00446823454094</v>
+        <v>2013.904666833063</v>
       </c>
       <c r="E105" t="n">
-        <v>69.93892773461884</v>
+        <v>2013.904672798508</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>steam&amp;PS&amp;Google play</t>
+          <t>rent + communal</t>
         </is>
       </c>
       <c r="B106" s="2" t="n">
-        <v>45690</v>
+        <v>45772</v>
       </c>
       <c r="C106" t="n">
-        <v>26.25755673475683</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>7.742746544735352</v>
+        <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>44.58148849763104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B107" s="2" t="n">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="C107" t="n">
-        <v>97.28422734157175</v>
+        <v>568.7406253261232</v>
       </c>
       <c r="D107" t="n">
-        <v>57.48891682518846</v>
+        <v>568.7387168783041</v>
       </c>
       <c r="E107" t="n">
-        <v>137.6255622601493</v>
+        <v>568.7453982768285</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B108" s="2" t="n">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="C108" t="n">
-        <v>54.61585373988868</v>
+        <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>14.40679602924298</v>
+        <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>96.27136024992406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B109" s="2" t="n">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="C109" t="n">
-        <v>33.16946592808489</v>
+        <v>89.81300975508654</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>89.77677660815324</v>
       </c>
       <c r="E109" t="n">
-        <v>72.75162941467387</v>
+        <v>89.84846394731292</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B110" s="2" t="n">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="C110" t="n">
-        <v>10.47583090110965</v>
+        <v>225.841590307633</v>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>225.7859357581737</v>
       </c>
       <c r="E110" t="n">
-        <v>51.10545402670731</v>
+        <v>225.894865891891</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B111" s="2" t="n">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>207.7898032032181</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>207.7062090363582</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>207.8593397818213</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B112" s="2" t="n">
-        <v>45760</v>
+        <v>45766</v>
       </c>
       <c r="C112" t="n">
-        <v>0</v>
+        <v>475.1233192824751</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>475.0100200741135</v>
       </c>
       <c r="E112" t="n">
-        <v>22.87236592186738</v>
+        <v>475.2235607080138</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>beauty</t>
         </is>
       </c>
       <c r="B113" s="2" t="n">
-        <v>45761</v>
+        <v>45767</v>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>362.3345295230044</v>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>362.1909379562848</v>
       </c>
       <c r="E113" t="n">
-        <v>34.70918091539647</v>
+        <v>362.456977823629</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B114" s="2" t="n">
-        <v>45766</v>
+        <v>45764</v>
       </c>
       <c r="C114" t="n">
-        <v>19.49280606198096</v>
+        <v>0</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>114.0521827271119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B115" s="2" t="n">
-        <v>45767</v>
+        <v>45765</v>
       </c>
       <c r="C115" t="n">
-        <v>85.64569675166589</v>
+        <v>159.5686549815661</v>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>159.5413818619122</v>
       </c>
       <c r="E115" t="n">
-        <v>179.4718531251938</v>
+        <v>159.5968837098493</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B116" s="2" t="n">
-        <v>45768</v>
+        <v>45766</v>
       </c>
       <c r="C116" t="n">
-        <v>32.50326962946897</v>
+        <v>0</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>129.336320420591</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B117" s="2" t="n">
-        <v>45769</v>
+        <v>45767</v>
       </c>
       <c r="C117" t="n">
-        <v>79.91209304693521</v>
+        <v>206.5593556266958</v>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>206.4543971024052</v>
       </c>
       <c r="E117" t="n">
-        <v>177.0960700547264</v>
+        <v>206.6746839111789</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B118" s="2" t="n">
-        <v>45770</v>
+        <v>45768</v>
       </c>
       <c r="C118" t="n">
-        <v>116.5748627280553</v>
+        <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>21.77058692121181</v>
+        <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>202.420208661709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B119" s="2" t="n">
-        <v>45771</v>
+        <v>45769</v>
       </c>
       <c r="C119" t="n">
-        <v>141.0569344190066</v>
+        <v>477.9179987457518</v>
       </c>
       <c r="D119" t="n">
-        <v>38.9616045511756</v>
+        <v>477.6875734124139</v>
       </c>
       <c r="E119" t="n">
-        <v>237.7378318124738</v>
+        <v>478.1550244856793</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>clothes</t>
+          <t>shop (not groceries)</t>
         </is>
       </c>
       <c r="B120" s="2" t="n">
-        <v>45772</v>
+        <v>45770</v>
       </c>
       <c r="C120" t="n">
-        <v>197.2059308781794</v>
+        <v>482.9357156435442</v>
       </c>
       <c r="D120" t="n">
-        <v>102.5871962068438</v>
+        <v>482.6328332535542</v>
       </c>
       <c r="E120" t="n">
-        <v>296.1040839611852</v>
+        <v>483.2436370044653</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B121" s="2" t="n">
-        <v>45766</v>
+        <v>45756</v>
       </c>
       <c r="C121" t="n">
-        <v>24.47974940485902</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>24.47974936741409</v>
+        <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>24.47974944814679</v>
+        <v>22.62602584538019</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B122" s="2" t="n">
-        <v>45767</v>
+        <v>45757</v>
       </c>
       <c r="C122" t="n">
-        <v>31.85438101000838</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>31.85438096650568</v>
+        <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>31.85438104923341</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B123" s="2" t="n">
-        <v>45768</v>
+        <v>45758</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
@@ -2785,1806 +2785,609 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B124" s="2" t="n">
-        <v>45769</v>
+        <v>45759</v>
       </c>
       <c r="C124" t="n">
-        <v>40.8543863070648</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>40.85438626626358</v>
+        <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>40.85438635078255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B125" s="2" t="n">
-        <v>45770</v>
+        <v>45760</v>
       </c>
       <c r="C125" t="n">
-        <v>10.67144348909977</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>10.67144345002473</v>
+        <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>10.67144352705224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B126" s="2" t="n">
-        <v>45771</v>
+        <v>45761</v>
       </c>
       <c r="C126" t="n">
-        <v>244.8813201426907</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>244.8813201040141</v>
+        <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>244.8813201822665</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>phone, internet</t>
+          <t>present</t>
         </is>
       </c>
       <c r="B127" s="2" t="n">
-        <v>45772</v>
+        <v>45762</v>
       </c>
       <c r="C127" t="n">
-        <v>60.52592997801828</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>60.52592993538608</v>
+        <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>60.52593001726387</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B128" s="2" t="n">
         <v>45766</v>
       </c>
       <c r="C128" t="n">
-        <v>0</v>
+        <v>283.2052176645828</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>283.2052172431761</v>
       </c>
       <c r="E128" t="n">
-        <v>364.0063880880693</v>
+        <v>283.205218089211</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B129" s="2" t="n">
         <v>45767</v>
       </c>
       <c r="C129" t="n">
-        <v>484.7693232641495</v>
+        <v>564.8830237576661</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>564.8830233703678</v>
       </c>
       <c r="E129" t="n">
-        <v>1042.076806176488</v>
+        <v>564.8830241953052</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B130" s="2" t="n">
         <v>45768</v>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>859.8702872048973</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>859.8702867702361</v>
       </c>
       <c r="E130" t="n">
-        <v>441.9969220338999</v>
+        <v>859.870287628037</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B131" s="2" t="n">
         <v>45769</v>
       </c>
       <c r="C131" t="n">
-        <v>0</v>
+        <v>1162.585773208802</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>1162.585772791461</v>
       </c>
       <c r="E131" t="n">
-        <v>554.2095553254757</v>
+        <v>1162.585773606933</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B132" s="2" t="n">
         <v>45770</v>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>1467.157486855562</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>1467.157486459336</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>1467.157487264323</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B133" s="2" t="n">
         <v>45771</v>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>1767.558627096387</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>1767.558626627196</v>
       </c>
       <c r="E133" t="n">
-        <v>407.2309624136439</v>
+        <v>1767.558627524104</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>rent + communal</t>
+          <t>Ira transfer</t>
         </is>
       </c>
       <c r="B134" s="2" t="n">
         <v>45772</v>
       </c>
       <c r="C134" t="n">
-        <v>0</v>
+        <v>2057.745803554395</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>2057.745803133957</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>2057.745803952436</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B135" s="2" t="n">
-        <v>45761</v>
+        <v>45755</v>
       </c>
       <c r="C135" t="n">
-        <v>9.938695308886679</v>
+        <v>0</v>
       </c>
       <c r="D135" t="n">
         <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>61.8573907495723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B136" s="2" t="n">
-        <v>45762</v>
+        <v>45756</v>
       </c>
       <c r="C136" t="n">
-        <v>35.01245268779337</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>87.48395892084552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B137" s="2" t="n">
-        <v>45763</v>
+        <v>45757</v>
       </c>
       <c r="C137" t="n">
-        <v>61.61196081958531</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>8.531102249771134</v>
+        <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>115.3735871682718</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B138" s="2" t="n">
-        <v>45764</v>
+        <v>45758</v>
       </c>
       <c r="C138" t="n">
-        <v>72.99574741909899</v>
+        <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>14.47507410918495</v>
+        <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>125.2656971384999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B139" s="2" t="n">
-        <v>45765</v>
+        <v>45759</v>
       </c>
       <c r="C139" t="n">
-        <v>30.88788968528277</v>
+        <v>0</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>83.27285750558963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B140" s="2" t="n">
-        <v>45766</v>
+        <v>45760</v>
       </c>
       <c r="C140" t="n">
-        <v>46.34059984731547</v>
+        <v>0</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>101.0765475695253</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>beauty</t>
+          <t>car rent</t>
         </is>
       </c>
       <c r="B141" s="2" t="n">
-        <v>45767</v>
+        <v>45761</v>
       </c>
       <c r="C141" t="n">
-        <v>41.47730938985555</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>95.62188072892974</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B142" s="2" t="n">
-        <v>45549</v>
+        <v>45767</v>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>96.79525606164273</v>
       </c>
       <c r="D142" t="n">
-        <v>0</v>
+        <v>96.79229398254161</v>
       </c>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>96.79632524033862</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B143" s="2" t="n">
-        <v>45550</v>
+        <v>45768</v>
       </c>
       <c r="C143" t="n">
-        <v>1881.882730905762</v>
+        <v>117.8656959195492</v>
       </c>
       <c r="D143" t="n">
-        <v>1881.882730859879</v>
+        <v>117.8557551366477</v>
       </c>
       <c r="E143" t="n">
-        <v>1881.882730946721</v>
+        <v>117.8707182937039</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B144" s="2" t="n">
-        <v>45551</v>
+        <v>45769</v>
       </c>
       <c r="C144" t="n">
-        <v>2013.781100554653</v>
+        <v>246.7546716290405</v>
       </c>
       <c r="D144" t="n">
-        <v>2013.781100504628</v>
+        <v>246.7340729112504</v>
       </c>
       <c r="E144" t="n">
-        <v>2013.781100598148</v>
+        <v>246.7654449243798</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B145" s="2" t="n">
-        <v>45552</v>
+        <v>45770</v>
       </c>
       <c r="C145" t="n">
-        <v>5679.034192967318</v>
+        <v>353.8565028982767</v>
       </c>
       <c r="D145" t="n">
-        <v>5679.034192911434</v>
+        <v>353.8246460962048</v>
       </c>
       <c r="E145" t="n">
-        <v>5679.034193014302</v>
+        <v>353.8744629791358</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B146" s="2" t="n">
-        <v>45553</v>
+        <v>45771</v>
       </c>
       <c r="C146" t="n">
-        <v>2716.508436779812</v>
+        <v>337.792425795022</v>
       </c>
       <c r="D146" t="n">
-        <v>2716.508436722201</v>
+        <v>337.747498806834</v>
       </c>
       <c r="E146" t="n">
-        <v>2716.508436829336</v>
+        <v>337.8192142033848</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B147" s="2" t="n">
-        <v>45554</v>
+        <v>45772</v>
       </c>
       <c r="C147" t="n">
-        <v>2228.400956888775</v>
+        <v>187.4418652699692</v>
       </c>
       <c r="D147" t="n">
-        <v>2228.400956830154</v>
+        <v>187.3817686435683</v>
       </c>
       <c r="E147" t="n">
-        <v>2228.402918682757</v>
+        <v>187.47895138484</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>airplane tickets</t>
+          <t>gas</t>
         </is>
       </c>
       <c r="B148" s="2" t="n">
-        <v>45555</v>
+        <v>45773</v>
       </c>
       <c r="C148" t="n">
-        <v>1414.155764121164</v>
+        <v>432.4840195945744</v>
       </c>
       <c r="D148" t="n">
-        <v>1414.15575582019</v>
+        <v>432.4060461494048</v>
       </c>
       <c r="E148" t="n">
-        <v>1414.159886777076</v>
+        <v>432.5326125765628</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B149" s="2" t="n">
-        <v>45764</v>
+        <v>45767</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>2604.492207412884</v>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>2604.482429932687</v>
       </c>
       <c r="E149" t="n">
-        <v>64.52723858231366</v>
+        <v>2604.50286375097</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B150" s="2" t="n">
-        <v>45765</v>
+        <v>45768</v>
       </c>
       <c r="C150" t="n">
-        <v>0</v>
+        <v>134.2509429940528</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>134.2030751785933</v>
       </c>
       <c r="E150" t="n">
-        <v>69.2913196731368</v>
+        <v>134.2977066459233</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B151" s="2" t="n">
-        <v>45766</v>
+        <v>45769</v>
       </c>
       <c r="C151" t="n">
-        <v>10.22563879875857</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>91.97807247920242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B152" s="2" t="n">
-        <v>45767</v>
+        <v>45770</v>
       </c>
       <c r="C152" t="n">
-        <v>37.62860474797796</v>
+        <v>2354.801503061747</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>2354.620272051378</v>
       </c>
       <c r="E152" t="n">
-        <v>114.1195421632777</v>
+        <v>2354.981227483922</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B153" s="2" t="n">
-        <v>45768</v>
+        <v>45771</v>
       </c>
       <c r="C153" t="n">
-        <v>5.747600018949413</v>
+        <v>232.6962945327873</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>232.4375898659457</v>
       </c>
       <c r="E153" t="n">
-        <v>83.19906222176472</v>
+        <v>232.9540193558909</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B154" s="2" t="n">
-        <v>45769</v>
+        <v>45772</v>
       </c>
       <c r="C154" t="n">
-        <v>47.2810835937601</v>
+        <v>0</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>125.0402190303556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>shop (not groceries)</t>
+          <t>Mira activities</t>
         </is>
       </c>
       <c r="B155" s="2" t="n">
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C155" t="n">
-        <v>17.82941600934635</v>
+        <v>0</v>
       </c>
       <c r="D155" t="n">
         <v>0</v>
       </c>
       <c r="E155" t="n">
-        <v>92.87122770347129</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B156" s="2" t="n">
-        <v>45197</v>
-      </c>
-      <c r="C156" t="n">
-        <v>13.07120412175945</v>
-      </c>
-      <c r="D156" t="n">
-        <v>13.07120405682249</v>
-      </c>
-      <c r="E156" t="n">
-        <v>13.07120419069754</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B157" s="2" t="n">
-        <v>45198</v>
-      </c>
-      <c r="C157" t="n">
-        <v>0</v>
-      </c>
-      <c r="D157" t="n">
-        <v>0</v>
-      </c>
-      <c r="E157" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B158" s="2" t="n">
-        <v>45199</v>
-      </c>
-      <c r="C158" t="n">
-        <v>0</v>
-      </c>
-      <c r="D158" t="n">
-        <v>0</v>
-      </c>
-      <c r="E158" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B159" s="2" t="n">
-        <v>45200</v>
-      </c>
-      <c r="C159" t="n">
-        <v>0</v>
-      </c>
-      <c r="D159" t="n">
-        <v>0</v>
-      </c>
-      <c r="E159" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B160" s="2" t="n">
-        <v>45201</v>
-      </c>
-      <c r="C160" t="n">
-        <v>0</v>
-      </c>
-      <c r="D160" t="n">
-        <v>0</v>
-      </c>
-      <c r="E160" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B161" s="2" t="n">
-        <v>45202</v>
-      </c>
-      <c r="C161" t="n">
-        <v>0</v>
-      </c>
-      <c r="D161" t="n">
-        <v>0</v>
-      </c>
-      <c r="E161" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>psychologist</t>
-        </is>
-      </c>
-      <c r="B162" s="2" t="n">
-        <v>45203</v>
-      </c>
-      <c r="C162" t="n">
-        <v>0</v>
-      </c>
-      <c r="D162" t="n">
-        <v>0</v>
-      </c>
-      <c r="E162" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B163" s="2" t="n">
-        <v>45740</v>
-      </c>
-      <c r="C163" t="n">
-        <v>49.77848652793453</v>
-      </c>
-      <c r="D163" t="n">
-        <v>47.98406251477756</v>
-      </c>
-      <c r="E163" t="n">
-        <v>51.6604327259195</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B164" s="2" t="n">
-        <v>45741</v>
-      </c>
-      <c r="C164" t="n">
-        <v>48.24265608987426</v>
-      </c>
-      <c r="D164" t="n">
-        <v>46.40359480882968</v>
-      </c>
-      <c r="E164" t="n">
-        <v>50.16901775632182</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B165" s="2" t="n">
-        <v>45742</v>
-      </c>
-      <c r="C165" t="n">
-        <v>49.89348402866861</v>
-      </c>
-      <c r="D165" t="n">
-        <v>47.9100533569243</v>
-      </c>
-      <c r="E165" t="n">
-        <v>51.72900027094008</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B166" s="2" t="n">
-        <v>45743</v>
-      </c>
-      <c r="C166" t="n">
-        <v>47.80531423065753</v>
-      </c>
-      <c r="D166" t="n">
-        <v>45.8896988594218</v>
-      </c>
-      <c r="E166" t="n">
-        <v>49.65937635331779</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B167" s="2" t="n">
-        <v>45744</v>
-      </c>
-      <c r="C167" t="n">
-        <v>48.21458060545149</v>
-      </c>
-      <c r="D167" t="n">
-        <v>46.51288129354647</v>
-      </c>
-      <c r="E167" t="n">
-        <v>50.22100769141047</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B168" s="2" t="n">
-        <v>45745</v>
-      </c>
-      <c r="C168" t="n">
-        <v>48.82633422435806</v>
-      </c>
-      <c r="D168" t="n">
-        <v>47.0675188236708</v>
-      </c>
-      <c r="E168" t="n">
-        <v>50.62170647597735</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>public transport</t>
-        </is>
-      </c>
-      <c r="B169" s="2" t="n">
-        <v>45746</v>
-      </c>
-      <c r="C169" t="n">
-        <v>46.68886232615696</v>
-      </c>
-      <c r="D169" t="n">
-        <v>44.9087503954236</v>
-      </c>
-      <c r="E169" t="n">
-        <v>48.49588215306875</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B170" s="2" t="n">
-        <v>45604</v>
-      </c>
-      <c r="C170" t="n">
-        <v>0</v>
-      </c>
-      <c r="D170" t="n">
-        <v>0</v>
-      </c>
-      <c r="E170" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B171" s="2" t="n">
-        <v>45605</v>
-      </c>
-      <c r="C171" t="n">
-        <v>25.07804861770069</v>
-      </c>
-      <c r="D171" t="n">
-        <v>8.294732790443572</v>
-      </c>
-      <c r="E171" t="n">
-        <v>40.91068331685425</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B172" s="2" t="n">
-        <v>45606</v>
-      </c>
-      <c r="C172" t="n">
-        <v>0</v>
-      </c>
-      <c r="D172" t="n">
-        <v>0</v>
-      </c>
-      <c r="E172" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B173" s="2" t="n">
-        <v>45607</v>
-      </c>
-      <c r="C173" t="n">
-        <v>0</v>
-      </c>
-      <c r="D173" t="n">
-        <v>0</v>
-      </c>
-      <c r="E173" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B174" s="2" t="n">
-        <v>45608</v>
-      </c>
-      <c r="C174" t="n">
-        <v>0</v>
-      </c>
-      <c r="D174" t="n">
-        <v>0</v>
-      </c>
-      <c r="E174" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B175" s="2" t="n">
-        <v>45609</v>
-      </c>
-      <c r="C175" t="n">
-        <v>77.96108777741688</v>
-      </c>
-      <c r="D175" t="n">
-        <v>58.84493514176034</v>
-      </c>
-      <c r="E175" t="n">
-        <v>94.91353259426461</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>services</t>
-        </is>
-      </c>
-      <c r="B176" s="2" t="n">
-        <v>45610</v>
-      </c>
-      <c r="C176" t="n">
-        <v>125.6753764321502</v>
-      </c>
-      <c r="D176" t="n">
-        <v>108.6197375879796</v>
-      </c>
-      <c r="E176" t="n">
-        <v>141.9601830301279</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B177" s="2" t="n">
-        <v>45756</v>
-      </c>
-      <c r="C177" t="n">
-        <v>174.7665971872941</v>
-      </c>
-      <c r="D177" t="n">
-        <v>3.834480866891517</v>
-      </c>
-      <c r="E177" t="n">
-        <v>347.5489647255395</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B178" s="2" t="n">
-        <v>45757</v>
-      </c>
-      <c r="C178" t="n">
-        <v>111.1996417000275</v>
-      </c>
-      <c r="D178" t="n">
-        <v>0</v>
-      </c>
-      <c r="E178" t="n">
-        <v>289.6450417946127</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B179" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="C179" t="n">
-        <v>215.7655212433893</v>
-      </c>
-      <c r="D179" t="n">
-        <v>52.65906283226301</v>
-      </c>
-      <c r="E179" t="n">
-        <v>405.039873567045</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B180" s="2" t="n">
-        <v>45759</v>
-      </c>
-      <c r="C180" t="n">
-        <v>85.20459732361556</v>
-      </c>
-      <c r="D180" t="n">
-        <v>0</v>
-      </c>
-      <c r="E180" t="n">
-        <v>236.4658068526611</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B181" s="2" t="n">
-        <v>45760</v>
-      </c>
-      <c r="C181" t="n">
-        <v>33.9192829411443</v>
-      </c>
-      <c r="D181" t="n">
-        <v>0</v>
-      </c>
-      <c r="E181" t="n">
-        <v>205.2504015175965</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B182" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="C182" t="n">
-        <v>169.3649217269276</v>
-      </c>
-      <c r="D182" t="n">
-        <v>0</v>
-      </c>
-      <c r="E182" t="n">
-        <v>341.5362844955524</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B183" s="2" t="n">
-        <v>45762</v>
-      </c>
-      <c r="C183" t="n">
-        <v>198.1666482333269</v>
-      </c>
-      <c r="D183" t="n">
-        <v>27.10612867464031</v>
-      </c>
-      <c r="E183" t="n">
-        <v>363.9072953062222</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B184" s="2" t="n">
-        <v>45766</v>
-      </c>
-      <c r="C184" t="n">
-        <v>0</v>
-      </c>
-      <c r="D184" t="n">
-        <v>0</v>
-      </c>
-      <c r="E184" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B185" s="2" t="n">
-        <v>45767</v>
-      </c>
-      <c r="C185" t="n">
-        <v>0</v>
-      </c>
-      <c r="D185" t="n">
-        <v>0</v>
-      </c>
-      <c r="E185" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B186" s="2" t="n">
-        <v>45768</v>
-      </c>
-      <c r="C186" t="n">
-        <v>0</v>
-      </c>
-      <c r="D186" t="n">
-        <v>0</v>
-      </c>
-      <c r="E186" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B187" s="2" t="n">
-        <v>45769</v>
-      </c>
-      <c r="C187" t="n">
-        <v>0</v>
-      </c>
-      <c r="D187" t="n">
-        <v>0</v>
-      </c>
-      <c r="E187" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B188" s="2" t="n">
-        <v>45770</v>
-      </c>
-      <c r="C188" t="n">
-        <v>0</v>
-      </c>
-      <c r="D188" t="n">
-        <v>0</v>
-      </c>
-      <c r="E188" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B189" s="2" t="n">
-        <v>45771</v>
-      </c>
-      <c r="C189" t="n">
-        <v>0</v>
-      </c>
-      <c r="D189" t="n">
-        <v>0</v>
-      </c>
-      <c r="E189" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>Ira transfer</t>
-        </is>
-      </c>
-      <c r="B190" s="2" t="n">
-        <v>45772</v>
-      </c>
-      <c r="C190" t="n">
-        <v>0</v>
-      </c>
-      <c r="D190" t="n">
-        <v>0</v>
-      </c>
-      <c r="E190" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B191" s="2" t="n">
-        <v>45755</v>
-      </c>
-      <c r="C191" t="n">
-        <v>0</v>
-      </c>
-      <c r="D191" t="n">
-        <v>0</v>
-      </c>
-      <c r="E191" t="n">
-        <v>119.4900138735956</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B192" s="2" t="n">
-        <v>45756</v>
-      </c>
-      <c r="C192" t="n">
-        <v>0</v>
-      </c>
-      <c r="D192" t="n">
-        <v>0</v>
-      </c>
-      <c r="E192" t="n">
-        <v>58.00761972862582</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B193" s="2" t="n">
-        <v>45757</v>
-      </c>
-      <c r="C193" t="n">
-        <v>0</v>
-      </c>
-      <c r="D193" t="n">
-        <v>0</v>
-      </c>
-      <c r="E193" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B194" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="C194" t="n">
-        <v>5.193754469110274</v>
-      </c>
-      <c r="D194" t="n">
-        <v>0</v>
-      </c>
-      <c r="E194" t="n">
-        <v>176.1238576699996</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B195" s="2" t="n">
-        <v>45759</v>
-      </c>
-      <c r="C195" t="n">
-        <v>0</v>
-      </c>
-      <c r="D195" t="n">
-        <v>0</v>
-      </c>
-      <c r="E195" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B196" s="2" t="n">
-        <v>45760</v>
-      </c>
-      <c r="C196" t="n">
-        <v>0</v>
-      </c>
-      <c r="D196" t="n">
-        <v>0</v>
-      </c>
-      <c r="E196" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>car rent</t>
-        </is>
-      </c>
-      <c r="B197" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="C197" t="n">
-        <v>0</v>
-      </c>
-      <c r="D197" t="n">
-        <v>0</v>
-      </c>
-      <c r="E197" t="n">
-        <v>65.70937395188882</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B198" s="2" t="n">
-        <v>45755</v>
-      </c>
-      <c r="C198" t="n">
-        <v>0</v>
-      </c>
-      <c r="D198" t="n">
-        <v>0</v>
-      </c>
-      <c r="E198" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B199" s="2" t="n">
-        <v>45756</v>
-      </c>
-      <c r="C199" t="n">
-        <v>0</v>
-      </c>
-      <c r="D199" t="n">
-        <v>0</v>
-      </c>
-      <c r="E199" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B200" s="2" t="n">
-        <v>45757</v>
-      </c>
-      <c r="C200" t="n">
-        <v>12.47275704039206</v>
-      </c>
-      <c r="D200" t="n">
-        <v>12.47275703837184</v>
-      </c>
-      <c r="E200" t="n">
-        <v>12.47275704233013</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B201" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="C201" t="n">
-        <v>0</v>
-      </c>
-      <c r="D201" t="n">
-        <v>0</v>
-      </c>
-      <c r="E201" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B202" s="2" t="n">
-        <v>45759</v>
-      </c>
-      <c r="C202" t="n">
-        <v>0</v>
-      </c>
-      <c r="D202" t="n">
-        <v>0</v>
-      </c>
-      <c r="E202" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B203" s="2" t="n">
-        <v>45760</v>
-      </c>
-      <c r="C203" t="n">
-        <v>0</v>
-      </c>
-      <c r="D203" t="n">
-        <v>0</v>
-      </c>
-      <c r="E203" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>parking</t>
-        </is>
-      </c>
-      <c r="B204" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="C204" t="n">
-        <v>38.49476695373325</v>
-      </c>
-      <c r="D204" t="n">
-        <v>38.49410368894643</v>
-      </c>
-      <c r="E204" t="n">
-        <v>38.49492622445537</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B205" s="2" t="n">
-        <v>45767</v>
-      </c>
-      <c r="C205" t="n">
-        <v>87.77623429487352</v>
-      </c>
-      <c r="D205" t="n">
-        <v>68.01190253659001</v>
-      </c>
-      <c r="E205" t="n">
-        <v>107.7890126704185</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B206" s="2" t="n">
-        <v>45768</v>
-      </c>
-      <c r="C206" t="n">
-        <v>114.6912863569044</v>
-      </c>
-      <c r="D206" t="n">
-        <v>95.07295386151824</v>
-      </c>
-      <c r="E206" t="n">
-        <v>134.9148306413544</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B207" s="2" t="n">
-        <v>45769</v>
-      </c>
-      <c r="C207" t="n">
-        <v>124.2912120767949</v>
-      </c>
-      <c r="D207" t="n">
-        <v>103.2915408130549</v>
-      </c>
-      <c r="E207" t="n">
-        <v>144.1575173179387</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B208" s="2" t="n">
-        <v>45770</v>
-      </c>
-      <c r="C208" t="n">
-        <v>126.5792631970978</v>
-      </c>
-      <c r="D208" t="n">
-        <v>105.2808811849783</v>
-      </c>
-      <c r="E208" t="n">
-        <v>146.0903301397506</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B209" s="2" t="n">
-        <v>45771</v>
-      </c>
-      <c r="C209" t="n">
-        <v>116.5525391542757</v>
-      </c>
-      <c r="D209" t="n">
-        <v>96.31096491187338</v>
-      </c>
-      <c r="E209" t="n">
-        <v>138.6919588763375</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B210" s="2" t="n">
-        <v>45772</v>
-      </c>
-      <c r="C210" t="n">
-        <v>147.7905078888436</v>
-      </c>
-      <c r="D210" t="n">
-        <v>127.0045131215473</v>
-      </c>
-      <c r="E210" t="n">
-        <v>168.0260282113213</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-      <c r="B211" s="2" t="n">
-        <v>45773</v>
-      </c>
-      <c r="C211" t="n">
-        <v>168.5855299109148</v>
-      </c>
-      <c r="D211" t="n">
-        <v>148.9884814892147</v>
-      </c>
-      <c r="E211" t="n">
-        <v>190.0214793641172</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B212" s="2" t="n">
-        <v>45767</v>
-      </c>
-      <c r="C212" t="n">
-        <v>211.6538617457347</v>
-      </c>
-      <c r="D212" t="n">
-        <v>199.2465322739002</v>
-      </c>
-      <c r="E212" t="n">
-        <v>224.621203225531</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B213" s="2" t="n">
-        <v>45768</v>
-      </c>
-      <c r="C213" t="n">
-        <v>211.4435520913225</v>
-      </c>
-      <c r="D213" t="n">
-        <v>198.1772986278266</v>
-      </c>
-      <c r="E213" t="n">
-        <v>224.0105219408347</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B214" s="2" t="n">
-        <v>45769</v>
-      </c>
-      <c r="C214" t="n">
-        <v>175.842843989309</v>
-      </c>
-      <c r="D214" t="n">
-        <v>163.0141190817917</v>
-      </c>
-      <c r="E214" t="n">
-        <v>188.734326236556</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B215" s="2" t="n">
-        <v>45770</v>
-      </c>
-      <c r="C215" t="n">
-        <v>302.3678234320873</v>
-      </c>
-      <c r="D215" t="n">
-        <v>289.8295794325211</v>
-      </c>
-      <c r="E215" t="n">
-        <v>314.7793248661724</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B216" s="2" t="n">
-        <v>45771</v>
-      </c>
-      <c r="C216" t="n">
-        <v>231.4787608994972</v>
-      </c>
-      <c r="D216" t="n">
-        <v>219.0991681152744</v>
-      </c>
-      <c r="E216" t="n">
-        <v>243.9165497790115</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B217" s="2" t="n">
-        <v>45772</v>
-      </c>
-      <c r="C217" t="n">
-        <v>0</v>
-      </c>
-      <c r="D217" t="n">
-        <v>0</v>
-      </c>
-      <c r="E217" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>Mira activities</t>
-        </is>
-      </c>
-      <c r="B218" s="2" t="n">
-        <v>45773</v>
-      </c>
-      <c r="C218" t="n">
-        <v>190.7427904754518</v>
-      </c>
-      <c r="D218" t="n">
-        <v>178.2258067622311</v>
-      </c>
-      <c r="E218" t="n">
-        <v>202.7615905444867</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes to app.py and forecast_results.xlsx
</commit_message>
<xml_diff>
--- a/forecast_results.xlsx
+++ b/forecast_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E346"/>
+  <dimension ref="A1:C346"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,16 +453,6 @@
           <t>forecast</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>lower</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>upper</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,8 +466,6 @@
       <c r="C2" t="n">
         <v>26.075</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,8 +479,6 @@
       <c r="C3" t="n">
         <v>26.075</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -506,8 +492,6 @@
       <c r="C4" t="n">
         <v>26.075</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -521,8 +505,6 @@
       <c r="C5" t="n">
         <v>26.075</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -536,8 +518,6 @@
       <c r="C6" t="n">
         <v>26.075</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,8 +531,6 @@
       <c r="C7" t="n">
         <v>26.075</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -566,8 +544,6 @@
       <c r="C8" t="n">
         <v>26.075</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -581,8 +557,6 @@
       <c r="C9" t="n">
         <v>26.075</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -596,8 +570,6 @@
       <c r="C10" t="n">
         <v>26.075</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -611,8 +583,6 @@
       <c r="C11" t="n">
         <v>26.075</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -626,8 +596,6 @@
       <c r="C12" t="n">
         <v>26.075</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -641,8 +609,6 @@
       <c r="C13" t="n">
         <v>26.075</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -656,8 +622,6 @@
       <c r="C14" t="n">
         <v>26.075</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -671,8 +635,6 @@
       <c r="C15" t="n">
         <v>26.075</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -686,8 +648,6 @@
       <c r="C16" t="n">
         <v>26.075</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -699,10 +659,8 @@
         <v>45768</v>
       </c>
       <c r="C17" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -714,10 +672,8 @@
         <v>45769</v>
       </c>
       <c r="C18" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -729,10 +685,8 @@
         <v>45770</v>
       </c>
       <c r="C19" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -744,10 +698,8 @@
         <v>45771</v>
       </c>
       <c r="C20" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -759,10 +711,8 @@
         <v>45772</v>
       </c>
       <c r="C21" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -774,10 +724,8 @@
         <v>45773</v>
       </c>
       <c r="C22" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -789,10 +737,8 @@
         <v>45774</v>
       </c>
       <c r="C23" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -804,10 +750,8 @@
         <v>45775</v>
       </c>
       <c r="C24" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -819,10 +763,8 @@
         <v>45776</v>
       </c>
       <c r="C25" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -834,10 +776,8 @@
         <v>45777</v>
       </c>
       <c r="C26" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -849,10 +789,8 @@
         <v>45778</v>
       </c>
       <c r="C27" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -864,10 +802,8 @@
         <v>45779</v>
       </c>
       <c r="C28" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -879,10 +815,8 @@
         <v>45780</v>
       </c>
       <c r="C29" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -894,10 +828,8 @@
         <v>45781</v>
       </c>
       <c r="C30" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -909,10 +841,8 @@
         <v>45782</v>
       </c>
       <c r="C31" t="n">
-        <v>5.015333333333333</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -926,8 +856,6 @@
       <c r="C32" t="n">
         <v>0</v>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -941,8 +869,6 @@
       <c r="C33" t="n">
         <v>0</v>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -956,8 +882,6 @@
       <c r="C34" t="n">
         <v>0</v>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -971,8 +895,6 @@
       <c r="C35" t="n">
         <v>0</v>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -986,8 +908,6 @@
       <c r="C36" t="n">
         <v>0</v>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1001,8 +921,6 @@
       <c r="C37" t="n">
         <v>0</v>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1016,8 +934,6 @@
       <c r="C38" t="n">
         <v>0</v>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1031,8 +947,6 @@
       <c r="C39" t="n">
         <v>0</v>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1046,8 +960,6 @@
       <c r="C40" t="n">
         <v>0</v>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1061,8 +973,6 @@
       <c r="C41" t="n">
         <v>0</v>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1076,8 +986,6 @@
       <c r="C42" t="n">
         <v>0</v>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1091,8 +999,6 @@
       <c r="C43" t="n">
         <v>0</v>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1106,8 +1012,6 @@
       <c r="C44" t="n">
         <v>0</v>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1121,8 +1025,6 @@
       <c r="C45" t="n">
         <v>0</v>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1136,8 +1038,6 @@
       <c r="C46" t="n">
         <v>0</v>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1151,8 +1051,6 @@
       <c r="C47" t="n">
         <v>0</v>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1166,8 +1064,6 @@
       <c r="C48" t="n">
         <v>0</v>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1181,8 +1077,6 @@
       <c r="C49" t="n">
         <v>0</v>
       </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1196,8 +1090,6 @@
       <c r="C50" t="n">
         <v>0</v>
       </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1211,8 +1103,6 @@
       <c r="C51" t="n">
         <v>0</v>
       </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1226,8 +1116,6 @@
       <c r="C52" t="n">
         <v>0</v>
       </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1241,8 +1129,6 @@
       <c r="C53" t="n">
         <v>0</v>
       </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1256,8 +1142,6 @@
       <c r="C54" t="n">
         <v>0</v>
       </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1271,8 +1155,6 @@
       <c r="C55" t="n">
         <v>0</v>
       </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1286,8 +1168,6 @@
       <c r="C56" t="n">
         <v>0</v>
       </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1301,8 +1181,6 @@
       <c r="C57" t="n">
         <v>0</v>
       </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1316,8 +1194,6 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1331,8 +1207,6 @@
       <c r="C59" t="n">
         <v>0</v>
       </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1346,8 +1220,6 @@
       <c r="C60" t="n">
         <v>0</v>
       </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1361,8 +1233,6 @@
       <c r="C61" t="n">
         <v>0</v>
       </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1376,8 +1246,6 @@
       <c r="C62" t="n">
         <v>0</v>
       </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1391,8 +1259,6 @@
       <c r="C63" t="n">
         <v>0</v>
       </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1406,8 +1272,6 @@
       <c r="C64" t="n">
         <v>0</v>
       </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1421,8 +1285,6 @@
       <c r="C65" t="n">
         <v>0</v>
       </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1436,8 +1298,6 @@
       <c r="C66" t="n">
         <v>0</v>
       </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1451,8 +1311,6 @@
       <c r="C67" t="n">
         <v>0</v>
       </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1466,8 +1324,6 @@
       <c r="C68" t="n">
         <v>0</v>
       </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1481,8 +1337,6 @@
       <c r="C69" t="n">
         <v>0</v>
       </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1496,8 +1350,6 @@
       <c r="C70" t="n">
         <v>0</v>
       </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1511,8 +1363,6 @@
       <c r="C71" t="n">
         <v>0</v>
       </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1526,8 +1376,6 @@
       <c r="C72" t="n">
         <v>0</v>
       </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1541,8 +1389,6 @@
       <c r="C73" t="n">
         <v>0</v>
       </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1556,8 +1402,6 @@
       <c r="C74" t="n">
         <v>0</v>
       </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1571,8 +1415,6 @@
       <c r="C75" t="n">
         <v>0</v>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1586,8 +1428,6 @@
       <c r="C76" t="n">
         <v>0</v>
       </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1599,10 +1439,8 @@
         <v>45768</v>
       </c>
       <c r="C77" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1614,10 +1452,8 @@
         <v>45769</v>
       </c>
       <c r="C78" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1629,10 +1465,8 @@
         <v>45770</v>
       </c>
       <c r="C79" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1644,10 +1478,8 @@
         <v>45771</v>
       </c>
       <c r="C80" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1659,10 +1491,8 @@
         <v>45772</v>
       </c>
       <c r="C81" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1674,10 +1504,8 @@
         <v>45773</v>
       </c>
       <c r="C82" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1689,10 +1517,8 @@
         <v>45774</v>
       </c>
       <c r="C83" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1704,10 +1530,8 @@
         <v>45775</v>
       </c>
       <c r="C84" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1719,10 +1543,8 @@
         <v>45776</v>
       </c>
       <c r="C85" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1734,10 +1556,8 @@
         <v>45777</v>
       </c>
       <c r="C86" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1749,10 +1569,8 @@
         <v>45778</v>
       </c>
       <c r="C87" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1764,10 +1582,8 @@
         <v>45779</v>
       </c>
       <c r="C88" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1779,10 +1595,8 @@
         <v>45780</v>
       </c>
       <c r="C89" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1794,10 +1608,8 @@
         <v>45781</v>
       </c>
       <c r="C90" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1809,10 +1621,8 @@
         <v>45782</v>
       </c>
       <c r="C91" t="n">
-        <v>11.86833333333333</v>
-      </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1826,8 +1636,6 @@
       <c r="C92" t="n">
         <v>0</v>
       </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1841,8 +1649,6 @@
       <c r="C93" t="n">
         <v>0</v>
       </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1856,8 +1662,6 @@
       <c r="C94" t="n">
         <v>0</v>
       </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1871,8 +1675,6 @@
       <c r="C95" t="n">
         <v>0</v>
       </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1886,8 +1688,6 @@
       <c r="C96" t="n">
         <v>0</v>
       </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1901,8 +1701,6 @@
       <c r="C97" t="n">
         <v>0</v>
       </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1916,8 +1714,6 @@
       <c r="C98" t="n">
         <v>0</v>
       </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1931,8 +1727,6 @@
       <c r="C99" t="n">
         <v>0</v>
       </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1946,8 +1740,6 @@
       <c r="C100" t="n">
         <v>0</v>
       </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1961,8 +1753,6 @@
       <c r="C101" t="n">
         <v>0</v>
       </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1976,8 +1766,6 @@
       <c r="C102" t="n">
         <v>0</v>
       </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1991,8 +1779,6 @@
       <c r="C103" t="n">
         <v>0</v>
       </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2006,8 +1792,6 @@
       <c r="C104" t="n">
         <v>0</v>
       </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2021,8 +1805,6 @@
       <c r="C105" t="n">
         <v>0</v>
       </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2036,8 +1818,6 @@
       <c r="C106" t="n">
         <v>0</v>
       </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2051,8 +1831,6 @@
       <c r="C107" t="n">
         <v>0</v>
       </c>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2066,8 +1844,6 @@
       <c r="C108" t="n">
         <v>0</v>
       </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2081,8 +1857,6 @@
       <c r="C109" t="n">
         <v>0</v>
       </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2096,8 +1870,6 @@
       <c r="C110" t="n">
         <v>0</v>
       </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2111,8 +1883,6 @@
       <c r="C111" t="n">
         <v>0</v>
       </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2126,8 +1896,6 @@
       <c r="C112" t="n">
         <v>0</v>
       </c>
-      <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2141,8 +1909,6 @@
       <c r="C113" t="n">
         <v>0</v>
       </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2156,8 +1922,6 @@
       <c r="C114" t="n">
         <v>0</v>
       </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2171,8 +1935,6 @@
       <c r="C115" t="n">
         <v>0</v>
       </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2186,8 +1948,6 @@
       <c r="C116" t="n">
         <v>0</v>
       </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2201,8 +1961,6 @@
       <c r="C117" t="n">
         <v>0</v>
       </c>
-      <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2216,8 +1974,6 @@
       <c r="C118" t="n">
         <v>0</v>
       </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2231,8 +1987,6 @@
       <c r="C119" t="n">
         <v>0</v>
       </c>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2246,8 +2000,6 @@
       <c r="C120" t="n">
         <v>0</v>
       </c>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2261,8 +2013,6 @@
       <c r="C121" t="n">
         <v>0</v>
       </c>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2276,8 +2026,6 @@
       <c r="C122" t="n">
         <v>0</v>
       </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2291,8 +2039,6 @@
       <c r="C123" t="n">
         <v>0</v>
       </c>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2306,8 +2052,6 @@
       <c r="C124" t="n">
         <v>0</v>
       </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2321,8 +2065,6 @@
       <c r="C125" t="n">
         <v>0</v>
       </c>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2336,8 +2078,6 @@
       <c r="C126" t="n">
         <v>0</v>
       </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2351,8 +2091,6 @@
       <c r="C127" t="n">
         <v>0</v>
       </c>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2366,8 +2104,6 @@
       <c r="C128" t="n">
         <v>0</v>
       </c>
-      <c r="D128" t="inlineStr"/>
-      <c r="E128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2381,8 +2117,6 @@
       <c r="C129" t="n">
         <v>0</v>
       </c>
-      <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2396,8 +2130,6 @@
       <c r="C130" t="n">
         <v>0</v>
       </c>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2411,8 +2143,6 @@
       <c r="C131" t="n">
         <v>0</v>
       </c>
-      <c r="D131" t="inlineStr"/>
-      <c r="E131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2426,8 +2156,6 @@
       <c r="C132" t="n">
         <v>0</v>
       </c>
-      <c r="D132" t="inlineStr"/>
-      <c r="E132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2441,8 +2169,6 @@
       <c r="C133" t="n">
         <v>0</v>
       </c>
-      <c r="D133" t="inlineStr"/>
-      <c r="E133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2456,8 +2182,6 @@
       <c r="C134" t="n">
         <v>0</v>
       </c>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2471,8 +2195,6 @@
       <c r="C135" t="n">
         <v>0</v>
       </c>
-      <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2486,8 +2208,6 @@
       <c r="C136" t="n">
         <v>0</v>
       </c>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2501,8 +2221,6 @@
       <c r="C137" t="n">
         <v>0</v>
       </c>
-      <c r="D137" t="inlineStr"/>
-      <c r="E137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2516,8 +2234,6 @@
       <c r="C138" t="n">
         <v>0</v>
       </c>
-      <c r="D138" t="inlineStr"/>
-      <c r="E138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2531,8 +2247,6 @@
       <c r="C139" t="n">
         <v>0</v>
       </c>
-      <c r="D139" t="inlineStr"/>
-      <c r="E139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2546,8 +2260,6 @@
       <c r="C140" t="n">
         <v>0</v>
       </c>
-      <c r="D140" t="inlineStr"/>
-      <c r="E140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2561,8 +2273,6 @@
       <c r="C141" t="n">
         <v>0</v>
       </c>
-      <c r="D141" t="inlineStr"/>
-      <c r="E141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2576,8 +2286,6 @@
       <c r="C142" t="n">
         <v>0</v>
       </c>
-      <c r="D142" t="inlineStr"/>
-      <c r="E142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2591,8 +2299,6 @@
       <c r="C143" t="n">
         <v>0</v>
       </c>
-      <c r="D143" t="inlineStr"/>
-      <c r="E143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2606,8 +2312,6 @@
       <c r="C144" t="n">
         <v>0</v>
       </c>
-      <c r="D144" t="inlineStr"/>
-      <c r="E144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2621,8 +2325,6 @@
       <c r="C145" t="n">
         <v>0</v>
       </c>
-      <c r="D145" t="inlineStr"/>
-      <c r="E145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2636,8 +2338,6 @@
       <c r="C146" t="n">
         <v>0</v>
       </c>
-      <c r="D146" t="inlineStr"/>
-      <c r="E146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2651,8 +2351,6 @@
       <c r="C147" t="n">
         <v>0</v>
       </c>
-      <c r="D147" t="inlineStr"/>
-      <c r="E147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2666,8 +2364,6 @@
       <c r="C148" t="n">
         <v>0</v>
       </c>
-      <c r="D148" t="inlineStr"/>
-      <c r="E148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2681,8 +2377,6 @@
       <c r="C149" t="n">
         <v>0</v>
       </c>
-      <c r="D149" t="inlineStr"/>
-      <c r="E149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2696,8 +2390,6 @@
       <c r="C150" t="n">
         <v>0</v>
       </c>
-      <c r="D150" t="inlineStr"/>
-      <c r="E150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2711,8 +2403,6 @@
       <c r="C151" t="n">
         <v>0</v>
       </c>
-      <c r="D151" t="inlineStr"/>
-      <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2726,8 +2416,6 @@
       <c r="C152" t="n">
         <v>0</v>
       </c>
-      <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2741,8 +2429,6 @@
       <c r="C153" t="n">
         <v>0</v>
       </c>
-      <c r="D153" t="inlineStr"/>
-      <c r="E153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2756,8 +2442,6 @@
       <c r="C154" t="n">
         <v>0</v>
       </c>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2771,8 +2455,6 @@
       <c r="C155" t="n">
         <v>0</v>
       </c>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2786,8 +2468,6 @@
       <c r="C156" t="n">
         <v>0</v>
       </c>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2801,8 +2481,6 @@
       <c r="C157" t="n">
         <v>0</v>
       </c>
-      <c r="D157" t="inlineStr"/>
-      <c r="E157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2816,8 +2494,6 @@
       <c r="C158" t="n">
         <v>0</v>
       </c>
-      <c r="D158" t="inlineStr"/>
-      <c r="E158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2831,8 +2507,6 @@
       <c r="C159" t="n">
         <v>0</v>
       </c>
-      <c r="D159" t="inlineStr"/>
-      <c r="E159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2846,8 +2520,6 @@
       <c r="C160" t="n">
         <v>0</v>
       </c>
-      <c r="D160" t="inlineStr"/>
-      <c r="E160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2861,8 +2533,6 @@
       <c r="C161" t="n">
         <v>0</v>
       </c>
-      <c r="D161" t="inlineStr"/>
-      <c r="E161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2876,8 +2546,6 @@
       <c r="C162" t="n">
         <v>0</v>
       </c>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2891,8 +2559,6 @@
       <c r="C163" t="n">
         <v>0</v>
       </c>
-      <c r="D163" t="inlineStr"/>
-      <c r="E163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2906,8 +2572,6 @@
       <c r="C164" t="n">
         <v>0</v>
       </c>
-      <c r="D164" t="inlineStr"/>
-      <c r="E164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2921,8 +2585,6 @@
       <c r="C165" t="n">
         <v>0</v>
       </c>
-      <c r="D165" t="inlineStr"/>
-      <c r="E165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2936,8 +2598,6 @@
       <c r="C166" t="n">
         <v>0</v>
       </c>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2951,8 +2611,6 @@
       <c r="C167" t="n">
         <v>0</v>
       </c>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2966,8 +2624,6 @@
       <c r="C168" t="n">
         <v>0</v>
       </c>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2981,8 +2637,6 @@
       <c r="C169" t="n">
         <v>0</v>
       </c>
-      <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2996,8 +2650,6 @@
       <c r="C170" t="n">
         <v>0</v>
       </c>
-      <c r="D170" t="inlineStr"/>
-      <c r="E170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3011,8 +2663,6 @@
       <c r="C171" t="n">
         <v>0</v>
       </c>
-      <c r="D171" t="inlineStr"/>
-      <c r="E171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3026,8 +2676,6 @@
       <c r="C172" t="n">
         <v>0</v>
       </c>
-      <c r="D172" t="inlineStr"/>
-      <c r="E172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3041,8 +2689,6 @@
       <c r="C173" t="n">
         <v>0</v>
       </c>
-      <c r="D173" t="inlineStr"/>
-      <c r="E173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3056,8 +2702,6 @@
       <c r="C174" t="n">
         <v>0</v>
       </c>
-      <c r="D174" t="inlineStr"/>
-      <c r="E174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3071,8 +2715,6 @@
       <c r="C175" t="n">
         <v>0</v>
       </c>
-      <c r="D175" t="inlineStr"/>
-      <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3086,8 +2728,6 @@
       <c r="C176" t="n">
         <v>0</v>
       </c>
-      <c r="D176" t="inlineStr"/>
-      <c r="E176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3101,8 +2741,6 @@
       <c r="C177" t="n">
         <v>0</v>
       </c>
-      <c r="D177" t="inlineStr"/>
-      <c r="E177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -3116,8 +2754,6 @@
       <c r="C178" t="n">
         <v>0</v>
       </c>
-      <c r="D178" t="inlineStr"/>
-      <c r="E178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -3131,8 +2767,6 @@
       <c r="C179" t="n">
         <v>0</v>
       </c>
-      <c r="D179" t="inlineStr"/>
-      <c r="E179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -3146,8 +2780,6 @@
       <c r="C180" t="n">
         <v>0</v>
       </c>
-      <c r="D180" t="inlineStr"/>
-      <c r="E180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -3161,8 +2793,6 @@
       <c r="C181" t="n">
         <v>0</v>
       </c>
-      <c r="D181" t="inlineStr"/>
-      <c r="E181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -3176,8 +2806,6 @@
       <c r="C182" t="n">
         <v>842</v>
       </c>
-      <c r="D182" t="inlineStr"/>
-      <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -3191,8 +2819,6 @@
       <c r="C183" t="n">
         <v>0</v>
       </c>
-      <c r="D183" t="inlineStr"/>
-      <c r="E183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -3206,8 +2832,6 @@
       <c r="C184" t="n">
         <v>0</v>
       </c>
-      <c r="D184" t="inlineStr"/>
-      <c r="E184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -3221,8 +2845,6 @@
       <c r="C185" t="n">
         <v>0</v>
       </c>
-      <c r="D185" t="inlineStr"/>
-      <c r="E185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -3236,8 +2858,6 @@
       <c r="C186" t="n">
         <v>0</v>
       </c>
-      <c r="D186" t="inlineStr"/>
-      <c r="E186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -3251,8 +2871,6 @@
       <c r="C187" t="n">
         <v>0</v>
       </c>
-      <c r="D187" t="inlineStr"/>
-      <c r="E187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -3266,8 +2884,6 @@
       <c r="C188" t="n">
         <v>0</v>
       </c>
-      <c r="D188" t="inlineStr"/>
-      <c r="E188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -3281,8 +2897,6 @@
       <c r="C189" t="n">
         <v>0</v>
       </c>
-      <c r="D189" t="inlineStr"/>
-      <c r="E189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -3296,8 +2910,6 @@
       <c r="C190" t="n">
         <v>0</v>
       </c>
-      <c r="D190" t="inlineStr"/>
-      <c r="E190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -3311,8 +2923,6 @@
       <c r="C191" t="n">
         <v>0</v>
       </c>
-      <c r="D191" t="inlineStr"/>
-      <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -3326,8 +2936,6 @@
       <c r="C192" t="n">
         <v>0</v>
       </c>
-      <c r="D192" t="inlineStr"/>
-      <c r="E192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -3341,8 +2949,6 @@
       <c r="C193" t="n">
         <v>0</v>
       </c>
-      <c r="D193" t="inlineStr"/>
-      <c r="E193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -3356,8 +2962,6 @@
       <c r="C194" t="n">
         <v>0</v>
       </c>
-      <c r="D194" t="inlineStr"/>
-      <c r="E194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -3371,8 +2975,6 @@
       <c r="C195" t="n">
         <v>0</v>
       </c>
-      <c r="D195" t="inlineStr"/>
-      <c r="E195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -3386,8 +2988,6 @@
       <c r="C196" t="n">
         <v>0</v>
       </c>
-      <c r="D196" t="inlineStr"/>
-      <c r="E196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -3399,10 +2999,8 @@
         <v>45768</v>
       </c>
       <c r="C197" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D197" t="inlineStr"/>
-      <c r="E197" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -3414,10 +3012,8 @@
         <v>45769</v>
       </c>
       <c r="C198" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D198" t="inlineStr"/>
-      <c r="E198" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -3429,10 +3025,8 @@
         <v>45770</v>
       </c>
       <c r="C199" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D199" t="inlineStr"/>
-      <c r="E199" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -3444,10 +3038,8 @@
         <v>45771</v>
       </c>
       <c r="C200" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D200" t="inlineStr"/>
-      <c r="E200" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -3459,10 +3051,8 @@
         <v>45772</v>
       </c>
       <c r="C201" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D201" t="inlineStr"/>
-      <c r="E201" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -3474,10 +3064,8 @@
         <v>45773</v>
       </c>
       <c r="C202" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D202" t="inlineStr"/>
-      <c r="E202" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -3489,10 +3077,8 @@
         <v>45774</v>
       </c>
       <c r="C203" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D203" t="inlineStr"/>
-      <c r="E203" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -3504,10 +3090,8 @@
         <v>45775</v>
       </c>
       <c r="C204" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D204" t="inlineStr"/>
-      <c r="E204" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -3519,10 +3103,8 @@
         <v>45776</v>
       </c>
       <c r="C205" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D205" t="inlineStr"/>
-      <c r="E205" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -3534,10 +3116,8 @@
         <v>45777</v>
       </c>
       <c r="C206" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D206" t="inlineStr"/>
-      <c r="E206" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -3549,10 +3129,8 @@
         <v>45778</v>
       </c>
       <c r="C207" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D207" t="inlineStr"/>
-      <c r="E207" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -3564,10 +3142,8 @@
         <v>45779</v>
       </c>
       <c r="C208" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D208" t="inlineStr"/>
-      <c r="E208" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -3579,10 +3155,8 @@
         <v>45780</v>
       </c>
       <c r="C209" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D209" t="inlineStr"/>
-      <c r="E209" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -3594,10 +3168,8 @@
         <v>45781</v>
       </c>
       <c r="C210" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D210" t="inlineStr"/>
-      <c r="E210" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -3609,10 +3181,8 @@
         <v>45782</v>
       </c>
       <c r="C211" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D211" t="inlineStr"/>
-      <c r="E211" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -3626,8 +3196,6 @@
       <c r="C212" t="n">
         <v>0</v>
       </c>
-      <c r="D212" t="inlineStr"/>
-      <c r="E212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -3641,8 +3209,6 @@
       <c r="C213" t="n">
         <v>0</v>
       </c>
-      <c r="D213" t="inlineStr"/>
-      <c r="E213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -3656,8 +3222,6 @@
       <c r="C214" t="n">
         <v>0</v>
       </c>
-      <c r="D214" t="inlineStr"/>
-      <c r="E214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -3671,8 +3235,6 @@
       <c r="C215" t="n">
         <v>0</v>
       </c>
-      <c r="D215" t="inlineStr"/>
-      <c r="E215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -3686,8 +3248,6 @@
       <c r="C216" t="n">
         <v>0</v>
       </c>
-      <c r="D216" t="inlineStr"/>
-      <c r="E216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -3701,8 +3261,6 @@
       <c r="C217" t="n">
         <v>0</v>
       </c>
-      <c r="D217" t="inlineStr"/>
-      <c r="E217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -3716,8 +3274,6 @@
       <c r="C218" t="n">
         <v>0</v>
       </c>
-      <c r="D218" t="inlineStr"/>
-      <c r="E218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -3731,8 +3287,6 @@
       <c r="C219" t="n">
         <v>0</v>
       </c>
-      <c r="D219" t="inlineStr"/>
-      <c r="E219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -3746,8 +3300,6 @@
       <c r="C220" t="n">
         <v>0</v>
       </c>
-      <c r="D220" t="inlineStr"/>
-      <c r="E220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -3761,8 +3313,6 @@
       <c r="C221" t="n">
         <v>0</v>
       </c>
-      <c r="D221" t="inlineStr"/>
-      <c r="E221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -3776,8 +3326,6 @@
       <c r="C222" t="n">
         <v>0</v>
       </c>
-      <c r="D222" t="inlineStr"/>
-      <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -3791,8 +3339,6 @@
       <c r="C223" t="n">
         <v>0</v>
       </c>
-      <c r="D223" t="inlineStr"/>
-      <c r="E223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -3806,8 +3352,6 @@
       <c r="C224" t="n">
         <v>0</v>
       </c>
-      <c r="D224" t="inlineStr"/>
-      <c r="E224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -3821,8 +3365,6 @@
       <c r="C225" t="n">
         <v>0</v>
       </c>
-      <c r="D225" t="inlineStr"/>
-      <c r="E225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -3836,8 +3378,6 @@
       <c r="C226" t="n">
         <v>0</v>
       </c>
-      <c r="D226" t="inlineStr"/>
-      <c r="E226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -3851,8 +3391,6 @@
       <c r="C227" t="n">
         <v>0</v>
       </c>
-      <c r="D227" t="inlineStr"/>
-      <c r="E227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -3866,8 +3404,6 @@
       <c r="C228" t="n">
         <v>0</v>
       </c>
-      <c r="D228" t="inlineStr"/>
-      <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -3881,8 +3417,6 @@
       <c r="C229" t="n">
         <v>0</v>
       </c>
-      <c r="D229" t="inlineStr"/>
-      <c r="E229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -3896,8 +3430,6 @@
       <c r="C230" t="n">
         <v>0</v>
       </c>
-      <c r="D230" t="inlineStr"/>
-      <c r="E230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -3911,8 +3443,6 @@
       <c r="C231" t="n">
         <v>0</v>
       </c>
-      <c r="D231" t="inlineStr"/>
-      <c r="E231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -3926,8 +3456,6 @@
       <c r="C232" t="n">
         <v>0</v>
       </c>
-      <c r="D232" t="inlineStr"/>
-      <c r="E232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -3941,8 +3469,6 @@
       <c r="C233" t="n">
         <v>0</v>
       </c>
-      <c r="D233" t="inlineStr"/>
-      <c r="E233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -3956,8 +3482,6 @@
       <c r="C234" t="n">
         <v>0</v>
       </c>
-      <c r="D234" t="inlineStr"/>
-      <c r="E234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -3971,8 +3495,6 @@
       <c r="C235" t="n">
         <v>0</v>
       </c>
-      <c r="D235" t="inlineStr"/>
-      <c r="E235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -3986,8 +3508,6 @@
       <c r="C236" t="n">
         <v>0</v>
       </c>
-      <c r="D236" t="inlineStr"/>
-      <c r="E236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -4001,8 +3521,6 @@
       <c r="C237" t="n">
         <v>0</v>
       </c>
-      <c r="D237" t="inlineStr"/>
-      <c r="E237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -4016,8 +3534,6 @@
       <c r="C238" t="n">
         <v>0</v>
       </c>
-      <c r="D238" t="inlineStr"/>
-      <c r="E238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -4031,8 +3547,6 @@
       <c r="C239" t="n">
         <v>0</v>
       </c>
-      <c r="D239" t="inlineStr"/>
-      <c r="E239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -4046,8 +3560,6 @@
       <c r="C240" t="n">
         <v>0</v>
       </c>
-      <c r="D240" t="inlineStr"/>
-      <c r="E240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -4061,8 +3573,6 @@
       <c r="C241" t="n">
         <v>0</v>
       </c>
-      <c r="D241" t="inlineStr"/>
-      <c r="E241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -4076,8 +3586,6 @@
       <c r="C242" t="n">
         <v>0</v>
       </c>
-      <c r="D242" t="inlineStr"/>
-      <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -4091,8 +3599,6 @@
       <c r="C243" t="n">
         <v>0</v>
       </c>
-      <c r="D243" t="inlineStr"/>
-      <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -4106,8 +3612,6 @@
       <c r="C244" t="n">
         <v>0</v>
       </c>
-      <c r="D244" t="inlineStr"/>
-      <c r="E244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -4121,8 +3625,6 @@
       <c r="C245" t="n">
         <v>0</v>
       </c>
-      <c r="D245" t="inlineStr"/>
-      <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -4136,8 +3638,6 @@
       <c r="C246" t="n">
         <v>0</v>
       </c>
-      <c r="D246" t="inlineStr"/>
-      <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -4151,8 +3651,6 @@
       <c r="C247" t="n">
         <v>0</v>
       </c>
-      <c r="D247" t="inlineStr"/>
-      <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -4166,8 +3664,6 @@
       <c r="C248" t="n">
         <v>0</v>
       </c>
-      <c r="D248" t="inlineStr"/>
-      <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -4181,8 +3677,6 @@
       <c r="C249" t="n">
         <v>0</v>
       </c>
-      <c r="D249" t="inlineStr"/>
-      <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -4196,8 +3690,6 @@
       <c r="C250" t="n">
         <v>0</v>
       </c>
-      <c r="D250" t="inlineStr"/>
-      <c r="E250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -4211,8 +3703,6 @@
       <c r="C251" t="n">
         <v>0</v>
       </c>
-      <c r="D251" t="inlineStr"/>
-      <c r="E251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -4226,8 +3716,6 @@
       <c r="C252" t="n">
         <v>0</v>
       </c>
-      <c r="D252" t="inlineStr"/>
-      <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -4241,8 +3729,6 @@
       <c r="C253" t="n">
         <v>0</v>
       </c>
-      <c r="D253" t="inlineStr"/>
-      <c r="E253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -4256,8 +3742,6 @@
       <c r="C254" t="n">
         <v>0</v>
       </c>
-      <c r="D254" t="inlineStr"/>
-      <c r="E254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -4271,8 +3755,6 @@
       <c r="C255" t="n">
         <v>0</v>
       </c>
-      <c r="D255" t="inlineStr"/>
-      <c r="E255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -4286,8 +3768,6 @@
       <c r="C256" t="n">
         <v>0</v>
       </c>
-      <c r="D256" t="inlineStr"/>
-      <c r="E256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -4301,8 +3781,6 @@
       <c r="C257" t="n">
         <v>0</v>
       </c>
-      <c r="D257" t="inlineStr"/>
-      <c r="E257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -4316,8 +3794,6 @@
       <c r="C258" t="n">
         <v>0</v>
       </c>
-      <c r="D258" t="inlineStr"/>
-      <c r="E258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -4331,8 +3807,6 @@
       <c r="C259" t="n">
         <v>0</v>
       </c>
-      <c r="D259" t="inlineStr"/>
-      <c r="E259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -4346,8 +3820,6 @@
       <c r="C260" t="n">
         <v>0</v>
       </c>
-      <c r="D260" t="inlineStr"/>
-      <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -4361,8 +3833,6 @@
       <c r="C261" t="n">
         <v>0</v>
       </c>
-      <c r="D261" t="inlineStr"/>
-      <c r="E261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -4376,8 +3846,6 @@
       <c r="C262" t="n">
         <v>0</v>
       </c>
-      <c r="D262" t="inlineStr"/>
-      <c r="E262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -4391,8 +3859,6 @@
       <c r="C263" t="n">
         <v>0</v>
       </c>
-      <c r="D263" t="inlineStr"/>
-      <c r="E263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -4406,8 +3872,6 @@
       <c r="C264" t="n">
         <v>0</v>
       </c>
-      <c r="D264" t="inlineStr"/>
-      <c r="E264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -4421,8 +3885,6 @@
       <c r="C265" t="n">
         <v>0</v>
       </c>
-      <c r="D265" t="inlineStr"/>
-      <c r="E265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -4436,8 +3898,6 @@
       <c r="C266" t="n">
         <v>0</v>
       </c>
-      <c r="D266" t="inlineStr"/>
-      <c r="E266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -4451,8 +3911,6 @@
       <c r="C267" t="n">
         <v>0</v>
       </c>
-      <c r="D267" t="inlineStr"/>
-      <c r="E267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -4466,8 +3924,6 @@
       <c r="C268" t="n">
         <v>0</v>
       </c>
-      <c r="D268" t="inlineStr"/>
-      <c r="E268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -4481,8 +3937,6 @@
       <c r="C269" t="n">
         <v>0</v>
       </c>
-      <c r="D269" t="inlineStr"/>
-      <c r="E269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -4496,8 +3950,6 @@
       <c r="C270" t="n">
         <v>0</v>
       </c>
-      <c r="D270" t="inlineStr"/>
-      <c r="E270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -4511,8 +3963,6 @@
       <c r="C271" t="n">
         <v>0</v>
       </c>
-      <c r="D271" t="inlineStr"/>
-      <c r="E271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -4524,10 +3974,8 @@
         <v>45768</v>
       </c>
       <c r="C272" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D272" t="inlineStr"/>
-      <c r="E272" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -4539,10 +3987,8 @@
         <v>45769</v>
       </c>
       <c r="C273" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D273" t="inlineStr"/>
-      <c r="E273" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -4554,10 +4000,8 @@
         <v>45770</v>
       </c>
       <c r="C274" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D274" t="inlineStr"/>
-      <c r="E274" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -4569,10 +4013,8 @@
         <v>45771</v>
       </c>
       <c r="C275" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D275" t="inlineStr"/>
-      <c r="E275" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -4584,10 +4026,8 @@
         <v>45772</v>
       </c>
       <c r="C276" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D276" t="inlineStr"/>
-      <c r="E276" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -4599,10 +4039,8 @@
         <v>45773</v>
       </c>
       <c r="C277" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D277" t="inlineStr"/>
-      <c r="E277" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -4614,10 +4052,8 @@
         <v>45774</v>
       </c>
       <c r="C278" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D278" t="inlineStr"/>
-      <c r="E278" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -4629,10 +4065,8 @@
         <v>45775</v>
       </c>
       <c r="C279" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D279" t="inlineStr"/>
-      <c r="E279" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -4644,10 +4078,8 @@
         <v>45776</v>
       </c>
       <c r="C280" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D280" t="inlineStr"/>
-      <c r="E280" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -4659,10 +4091,8 @@
         <v>45777</v>
       </c>
       <c r="C281" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D281" t="inlineStr"/>
-      <c r="E281" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -4674,10 +4104,8 @@
         <v>45778</v>
       </c>
       <c r="C282" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D282" t="inlineStr"/>
-      <c r="E282" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -4689,10 +4117,8 @@
         <v>45779</v>
       </c>
       <c r="C283" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D283" t="inlineStr"/>
-      <c r="E283" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -4704,10 +4130,8 @@
         <v>45780</v>
       </c>
       <c r="C284" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D284" t="inlineStr"/>
-      <c r="E284" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -4719,10 +4143,8 @@
         <v>45781</v>
       </c>
       <c r="C285" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D285" t="inlineStr"/>
-      <c r="E285" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -4734,10 +4156,8 @@
         <v>45782</v>
       </c>
       <c r="C286" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D286" t="inlineStr"/>
-      <c r="E286" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -4751,8 +4171,6 @@
       <c r="C287" t="n">
         <v>0</v>
       </c>
-      <c r="D287" t="inlineStr"/>
-      <c r="E287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -4766,8 +4184,6 @@
       <c r="C288" t="n">
         <v>0</v>
       </c>
-      <c r="D288" t="inlineStr"/>
-      <c r="E288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -4781,8 +4197,6 @@
       <c r="C289" t="n">
         <v>0</v>
       </c>
-      <c r="D289" t="inlineStr"/>
-      <c r="E289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -4796,8 +4210,6 @@
       <c r="C290" t="n">
         <v>0</v>
       </c>
-      <c r="D290" t="inlineStr"/>
-      <c r="E290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -4811,8 +4223,6 @@
       <c r="C291" t="n">
         <v>0</v>
       </c>
-      <c r="D291" t="inlineStr"/>
-      <c r="E291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -4826,8 +4236,6 @@
       <c r="C292" t="n">
         <v>0</v>
       </c>
-      <c r="D292" t="inlineStr"/>
-      <c r="E292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -4841,8 +4249,6 @@
       <c r="C293" t="n">
         <v>0</v>
       </c>
-      <c r="D293" t="inlineStr"/>
-      <c r="E293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -4856,8 +4262,6 @@
       <c r="C294" t="n">
         <v>0</v>
       </c>
-      <c r="D294" t="inlineStr"/>
-      <c r="E294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -4871,8 +4275,6 @@
       <c r="C295" t="n">
         <v>0</v>
       </c>
-      <c r="D295" t="inlineStr"/>
-      <c r="E295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -4886,8 +4288,6 @@
       <c r="C296" t="n">
         <v>0</v>
       </c>
-      <c r="D296" t="inlineStr"/>
-      <c r="E296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -4901,8 +4301,6 @@
       <c r="C297" t="n">
         <v>0</v>
       </c>
-      <c r="D297" t="inlineStr"/>
-      <c r="E297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -4916,8 +4314,6 @@
       <c r="C298" t="n">
         <v>0</v>
       </c>
-      <c r="D298" t="inlineStr"/>
-      <c r="E298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -4931,8 +4327,6 @@
       <c r="C299" t="n">
         <v>0</v>
       </c>
-      <c r="D299" t="inlineStr"/>
-      <c r="E299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -4946,8 +4340,6 @@
       <c r="C300" t="n">
         <v>0</v>
       </c>
-      <c r="D300" t="inlineStr"/>
-      <c r="E300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -4961,8 +4353,6 @@
       <c r="C301" t="n">
         <v>0</v>
       </c>
-      <c r="D301" t="inlineStr"/>
-      <c r="E301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -4976,8 +4366,6 @@
       <c r="C302" t="n">
         <v>0</v>
       </c>
-      <c r="D302" t="inlineStr"/>
-      <c r="E302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -4991,8 +4379,6 @@
       <c r="C303" t="n">
         <v>0</v>
       </c>
-      <c r="D303" t="inlineStr"/>
-      <c r="E303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -5006,8 +4392,6 @@
       <c r="C304" t="n">
         <v>0</v>
       </c>
-      <c r="D304" t="inlineStr"/>
-      <c r="E304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -5021,8 +4405,6 @@
       <c r="C305" t="n">
         <v>0</v>
       </c>
-      <c r="D305" t="inlineStr"/>
-      <c r="E305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -5036,8 +4418,6 @@
       <c r="C306" t="n">
         <v>0</v>
       </c>
-      <c r="D306" t="inlineStr"/>
-      <c r="E306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -5051,8 +4431,6 @@
       <c r="C307" t="n">
         <v>0</v>
       </c>
-      <c r="D307" t="inlineStr"/>
-      <c r="E307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -5066,8 +4444,6 @@
       <c r="C308" t="n">
         <v>0</v>
       </c>
-      <c r="D308" t="inlineStr"/>
-      <c r="E308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -5081,8 +4457,6 @@
       <c r="C309" t="n">
         <v>0</v>
       </c>
-      <c r="D309" t="inlineStr"/>
-      <c r="E309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -5096,8 +4470,6 @@
       <c r="C310" t="n">
         <v>0</v>
       </c>
-      <c r="D310" t="inlineStr"/>
-      <c r="E310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -5111,8 +4483,6 @@
       <c r="C311" t="n">
         <v>0</v>
       </c>
-      <c r="D311" t="inlineStr"/>
-      <c r="E311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -5126,8 +4496,6 @@
       <c r="C312" t="n">
         <v>0</v>
       </c>
-      <c r="D312" t="inlineStr"/>
-      <c r="E312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -5141,8 +4509,6 @@
       <c r="C313" t="n">
         <v>0</v>
       </c>
-      <c r="D313" t="inlineStr"/>
-      <c r="E313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -5156,8 +4522,6 @@
       <c r="C314" t="n">
         <v>0</v>
       </c>
-      <c r="D314" t="inlineStr"/>
-      <c r="E314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -5171,8 +4535,6 @@
       <c r="C315" t="n">
         <v>0</v>
       </c>
-      <c r="D315" t="inlineStr"/>
-      <c r="E315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -5186,8 +4548,6 @@
       <c r="C316" t="n">
         <v>0</v>
       </c>
-      <c r="D316" t="inlineStr"/>
-      <c r="E316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -5201,8 +4561,6 @@
       <c r="C317" t="n">
         <v>0</v>
       </c>
-      <c r="D317" t="inlineStr"/>
-      <c r="E317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -5216,8 +4574,6 @@
       <c r="C318" t="n">
         <v>0</v>
       </c>
-      <c r="D318" t="inlineStr"/>
-      <c r="E318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -5231,8 +4587,6 @@
       <c r="C319" t="n">
         <v>0</v>
       </c>
-      <c r="D319" t="inlineStr"/>
-      <c r="E319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -5246,8 +4600,6 @@
       <c r="C320" t="n">
         <v>0</v>
       </c>
-      <c r="D320" t="inlineStr"/>
-      <c r="E320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -5261,8 +4613,6 @@
       <c r="C321" t="n">
         <v>0</v>
       </c>
-      <c r="D321" t="inlineStr"/>
-      <c r="E321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -5276,8 +4626,6 @@
       <c r="C322" t="n">
         <v>0</v>
       </c>
-      <c r="D322" t="inlineStr"/>
-      <c r="E322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -5291,8 +4639,6 @@
       <c r="C323" t="n">
         <v>0</v>
       </c>
-      <c r="D323" t="inlineStr"/>
-      <c r="E323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -5306,8 +4652,6 @@
       <c r="C324" t="n">
         <v>0</v>
       </c>
-      <c r="D324" t="inlineStr"/>
-      <c r="E324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -5321,8 +4665,6 @@
       <c r="C325" t="n">
         <v>0</v>
       </c>
-      <c r="D325" t="inlineStr"/>
-      <c r="E325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -5336,8 +4678,6 @@
       <c r="C326" t="n">
         <v>0</v>
       </c>
-      <c r="D326" t="inlineStr"/>
-      <c r="E326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -5351,8 +4691,6 @@
       <c r="C327" t="n">
         <v>0</v>
       </c>
-      <c r="D327" t="inlineStr"/>
-      <c r="E327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -5366,8 +4704,6 @@
       <c r="C328" t="n">
         <v>0</v>
       </c>
-      <c r="D328" t="inlineStr"/>
-      <c r="E328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -5381,8 +4717,6 @@
       <c r="C329" t="n">
         <v>0</v>
       </c>
-      <c r="D329" t="inlineStr"/>
-      <c r="E329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -5396,8 +4730,6 @@
       <c r="C330" t="n">
         <v>0</v>
       </c>
-      <c r="D330" t="inlineStr"/>
-      <c r="E330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -5411,8 +4743,6 @@
       <c r="C331" t="n">
         <v>0</v>
       </c>
-      <c r="D331" t="inlineStr"/>
-      <c r="E331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -5426,8 +4756,6 @@
       <c r="C332" t="n">
         <v>0</v>
       </c>
-      <c r="D332" t="inlineStr"/>
-      <c r="E332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -5441,8 +4769,6 @@
       <c r="C333" t="n">
         <v>0</v>
       </c>
-      <c r="D333" t="inlineStr"/>
-      <c r="E333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -5456,8 +4782,6 @@
       <c r="C334" t="n">
         <v>0</v>
       </c>
-      <c r="D334" t="inlineStr"/>
-      <c r="E334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -5471,8 +4795,6 @@
       <c r="C335" t="n">
         <v>0</v>
       </c>
-      <c r="D335" t="inlineStr"/>
-      <c r="E335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -5486,8 +4808,6 @@
       <c r="C336" t="n">
         <v>0</v>
       </c>
-      <c r="D336" t="inlineStr"/>
-      <c r="E336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -5499,10 +4819,8 @@
         <v>45773</v>
       </c>
       <c r="C337" t="n">
-        <v>12.77</v>
-      </c>
-      <c r="D337" t="inlineStr"/>
-      <c r="E337" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -5516,8 +4834,6 @@
       <c r="C338" t="n">
         <v>0</v>
       </c>
-      <c r="D338" t="inlineStr"/>
-      <c r="E338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -5531,8 +4847,6 @@
       <c r="C339" t="n">
         <v>0</v>
       </c>
-      <c r="D339" t="inlineStr"/>
-      <c r="E339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -5546,8 +4860,6 @@
       <c r="C340" t="n">
         <v>0</v>
       </c>
-      <c r="D340" t="inlineStr"/>
-      <c r="E340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -5561,8 +4873,6 @@
       <c r="C341" t="n">
         <v>0</v>
       </c>
-      <c r="D341" t="inlineStr"/>
-      <c r="E341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -5576,8 +4886,6 @@
       <c r="C342" t="n">
         <v>0</v>
       </c>
-      <c r="D342" t="inlineStr"/>
-      <c r="E342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -5591,8 +4899,6 @@
       <c r="C343" t="n">
         <v>0</v>
       </c>
-      <c r="D343" t="inlineStr"/>
-      <c r="E343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -5606,8 +4912,6 @@
       <c r="C344" t="n">
         <v>0</v>
       </c>
-      <c r="D344" t="inlineStr"/>
-      <c r="E344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -5621,8 +4925,6 @@
       <c r="C345" t="n">
         <v>0</v>
       </c>
-      <c r="D345" t="inlineStr"/>
-      <c r="E345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -5636,8 +4938,6 @@
       <c r="C346" t="n">
         <v>0</v>
       </c>
-      <c r="D346" t="inlineStr"/>
-      <c r="E346" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update codebase with latest changes including UI modularization and forecast metrics improvements
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/forecast_results.xlsx
+++ b/forecast_results.xlsx
@@ -464,7 +464,7 @@
         <v>45863</v>
       </c>
       <c r="C2" t="n">
-        <v>33.7285886159742</v>
+        <v>41.90542479266645</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         <v>45864</v>
       </c>
       <c r="C3" t="n">
-        <v>39.03984043145672</v>
+        <v>38.49402873427938</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>45865</v>
       </c>
       <c r="C4" t="n">
-        <v>8.801180051587268</v>
+        <v>6.425165193507417</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         <v>45866</v>
       </c>
       <c r="C5" t="n">
-        <v>48.3073919398682</v>
+        <v>47.09297571453026</v>
       </c>
     </row>
     <row r="6">
@@ -516,7 +516,7 @@
         <v>45867</v>
       </c>
       <c r="C6" t="n">
-        <v>38.53995634831496</v>
+        <v>40.73434009058274</v>
       </c>
     </row>
     <row r="7">
@@ -529,7 +529,7 @@
         <v>45868</v>
       </c>
       <c r="C7" t="n">
-        <v>43.85792228928054</v>
+        <v>47.95405382554818</v>
       </c>
     </row>
     <row r="8">
@@ -542,7 +542,7 @@
         <v>45869</v>
       </c>
       <c r="C8" t="n">
-        <v>44.39438612824315</v>
+        <v>44.18388664128612</v>
       </c>
     </row>
     <row r="9">
@@ -568,7 +568,7 @@
         <v>45864</v>
       </c>
       <c r="C10" t="n">
-        <v>36.45041950800235</v>
+        <v>36.05412462389766</v>
       </c>
     </row>
     <row r="11">
@@ -581,7 +581,7 @@
         <v>45865</v>
       </c>
       <c r="C11" t="n">
-        <v>22.52496801570798</v>
+        <v>22.6026861500278</v>
       </c>
     </row>
     <row r="12">
@@ -594,7 +594,7 @@
         <v>45866</v>
       </c>
       <c r="C12" t="n">
-        <v>1.140786095189984</v>
+        <v>1.500250415078458</v>
       </c>
     </row>
     <row r="13">
@@ -607,7 +607,7 @@
         <v>45867</v>
       </c>
       <c r="C13" t="n">
-        <v>0.326073436613155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -633,7 +633,7 @@
         <v>45869</v>
       </c>
       <c r="C15" t="n">
-        <v>4.094147680108867</v>
+        <v>4.65795748237634</v>
       </c>
     </row>
     <row r="16">
@@ -1647,7 +1647,7 @@
         <v>45863</v>
       </c>
       <c r="C93" t="n">
-        <v>0.0673803069389582</v>
+        <v>0.08146223558543657</v>
       </c>
     </row>
     <row r="94">
@@ -1660,7 +1660,7 @@
         <v>45864</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>0.01615361644590407</v>
       </c>
     </row>
     <row r="95">
@@ -1673,7 +1673,7 @@
         <v>45865</v>
       </c>
       <c r="C95" t="n">
-        <v>2.084093141159541</v>
+        <v>2.097005524008066</v>
       </c>
     </row>
     <row r="96">
@@ -1686,7 +1686,7 @@
         <v>45866</v>
       </c>
       <c r="C96" t="n">
-        <v>0.0752336908640597</v>
+        <v>0.002014158141016677</v>
       </c>
     </row>
     <row r="97">
@@ -1699,7 +1699,7 @@
         <v>45867</v>
       </c>
       <c r="C97" t="n">
-        <v>1.159196887262711</v>
+        <v>1.144186650192057</v>
       </c>
     </row>
     <row r="98">
@@ -1712,7 +1712,7 @@
         <v>45868</v>
       </c>
       <c r="C98" t="n">
-        <v>1.031577911451526</v>
+        <v>1.259004036088275</v>
       </c>
     </row>
     <row r="99">
@@ -1725,7 +1725,7 @@
         <v>45869</v>
       </c>
       <c r="C99" t="n">
-        <v>0.04783655377309661</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -1738,7 +1738,7 @@
         <v>45863</v>
       </c>
       <c r="C100" t="n">
-        <v>7.446331095872016</v>
+        <v>7.511973968952613</v>
       </c>
     </row>
     <row r="101">
@@ -1751,7 +1751,7 @@
         <v>45864</v>
       </c>
       <c r="C101" t="n">
-        <v>0.5837523794174964</v>
+        <v>0.92962479075577</v>
       </c>
     </row>
     <row r="102">
@@ -1764,7 +1764,7 @@
         <v>45865</v>
       </c>
       <c r="C102" t="n">
-        <v>2.249894246604051</v>
+        <v>2.349444947102698</v>
       </c>
     </row>
     <row r="103">
@@ -1777,7 +1777,7 @@
         <v>45866</v>
       </c>
       <c r="C103" t="n">
-        <v>0.009259861259759665</v>
+        <v>0.06719329937135948</v>
       </c>
     </row>
     <row r="104">
@@ -1790,7 +1790,7 @@
         <v>45867</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1981251808089306</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -1803,7 +1803,7 @@
         <v>45868</v>
       </c>
       <c r="C105" t="n">
-        <v>0.2053204491752422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -1816,7 +1816,7 @@
         <v>45869</v>
       </c>
       <c r="C106" t="n">
-        <v>4.759414553207573</v>
+        <v>4.827966511230345</v>
       </c>
     </row>
     <row r="107">
@@ -1829,7 +1829,7 @@
         <v>45863</v>
       </c>
       <c r="C107" t="n">
-        <v>1.548957220853535</v>
+        <v>1.509224491614277</v>
       </c>
     </row>
     <row r="108">
@@ -1842,7 +1842,7 @@
         <v>45864</v>
       </c>
       <c r="C108" t="n">
-        <v>12.97948785432254</v>
+        <v>12.95482561237078</v>
       </c>
     </row>
     <row r="109">
@@ -1868,7 +1868,7 @@
         <v>45866</v>
       </c>
       <c r="C110" t="n">
-        <v>0.673890896375966</v>
+        <v>0.71157218845641</v>
       </c>
     </row>
     <row r="111">
@@ -1894,7 +1894,7 @@
         <v>45868</v>
       </c>
       <c r="C112" t="n">
-        <v>0.01157282758218413</v>
+        <v>0.1952368699170393</v>
       </c>
     </row>
     <row r="113">
@@ -1907,7 +1907,7 @@
         <v>45869</v>
       </c>
       <c r="C113" t="n">
-        <v>3.297598604791099</v>
+        <v>3.248394638311456</v>
       </c>
     </row>
     <row r="114">
@@ -2011,7 +2011,7 @@
         <v>45863</v>
       </c>
       <c r="C121" t="n">
-        <v>12.03227757330267</v>
+        <v>9.521895170679079</v>
       </c>
     </row>
     <row r="122">
@@ -2024,7 +2024,7 @@
         <v>45864</v>
       </c>
       <c r="C122" t="n">
-        <v>0</v>
+        <v>4.056154768915386</v>
       </c>
     </row>
     <row r="123">
@@ -2037,7 +2037,7 @@
         <v>45865</v>
       </c>
       <c r="C123" t="n">
-        <v>1.126081545623826</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -2050,7 +2050,7 @@
         <v>45866</v>
       </c>
       <c r="C124" t="n">
-        <v>0.5426503968743743</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -2063,7 +2063,7 @@
         <v>45867</v>
       </c>
       <c r="C125" t="n">
-        <v>178.6499685109372</v>
+        <v>179.8432663935019</v>
       </c>
     </row>
     <row r="126">
@@ -2076,7 +2076,7 @@
         <v>45868</v>
       </c>
       <c r="C126" t="n">
-        <v>4.485537683325485</v>
+        <v>3.034031357935503</v>
       </c>
     </row>
     <row r="127">
@@ -2089,7 +2089,7 @@
         <v>45869</v>
       </c>
       <c r="C127" t="n">
-        <v>60.08636034716793</v>
+        <v>63.31538421522037</v>
       </c>
     </row>
     <row r="128">

</xml_diff>